<commit_message>
Agrego Especificación de casos de Prueba + algunas pruebas
Las agregue porque nunca las había hecho y eran necesarias para la especificaición.
</commit_message>
<xml_diff>
--- a/docs/Casos de prueba.xlsx
+++ b/docs/Casos de prueba.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1703" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1754" uniqueCount="338">
   <si>
     <t>ID caso de prueba</t>
   </si>
@@ -943,6 +943,96 @@
   </si>
   <si>
     <t>sqlite3.IntegrityError: UNIQUE constraint failed: colaborador.idProyecto, colaborador.idUsuario</t>
+  </si>
+  <si>
+    <t>Escribir usuario "root"</t>
+  </si>
+  <si>
+    <t>Escribir contraseña "root"</t>
+  </si>
+  <si>
+    <t>Ingresar "data mining AND software and XML" y hacer click en Buscar</t>
+  </si>
+  <si>
+    <t>Seleccionar el artículo "Drafting and Retrieving…"</t>
+  </si>
+  <si>
+    <t>Usuario logeado, proyecto seleccionado y pantalla de búsqueda</t>
+  </si>
+  <si>
+    <t>Que el usuario pueda agregar artículos que encontró a su proyecto</t>
+  </si>
+  <si>
+    <t>Seleccionar el artículo "Application of XML Data Mining..."</t>
+  </si>
+  <si>
+    <t>Hacer click en "Agregar articulos seleccionados"</t>
+  </si>
+  <si>
+    <t>Scrapping - Agregar Articulos</t>
+  </si>
+  <si>
+    <t>Los articulos son eliminados de los resultados y agregados al proyecto</t>
+  </si>
+  <si>
+    <t>Proyecto creado, Artículos buscados y pantalla de clasificacion de proyectos</t>
+  </si>
+  <si>
+    <t>Que el usuario pueda clasificar los Articulos</t>
+  </si>
+  <si>
+    <t>PRS_0044</t>
+  </si>
+  <si>
+    <t>PRS_0043</t>
+  </si>
+  <si>
+    <t>Classify</t>
+  </si>
+  <si>
+    <t>Seleccionar un Artículo y clasificarlo como "Poca información"</t>
+  </si>
+  <si>
+    <t>Seleccionar otro Artículo y clasificarlo como "Relevante"</t>
+  </si>
+  <si>
+    <t>Hacer click en guardar en ambos artículos</t>
+  </si>
+  <si>
+    <t>Los artículos desaparecen de la lista</t>
+  </si>
+  <si>
+    <t>Recargar la pagina</t>
+  </si>
+  <si>
+    <t>Los artículos aparecen junto a la clasificación que se les dio</t>
+  </si>
+  <si>
+    <t>PRS_0045</t>
+  </si>
+  <si>
+    <t>PRS_0046</t>
+  </si>
+  <si>
+    <t>Que el usuario pueda modificar la clasificación que le asignó al Artículo</t>
+  </si>
+  <si>
+    <t>Proyecto creado, articulo clasificado y pantalla de clasificar artículos</t>
+  </si>
+  <si>
+    <t>Hacer click en la clasificacion que se le dio al artículo</t>
+  </si>
+  <si>
+    <t>Se abre una ventana que permite renombrar la clasificación</t>
+  </si>
+  <si>
+    <t>Cambiar "Relevante" por "No interesa"</t>
+  </si>
+  <si>
+    <t>Hacer click en "editar"</t>
+  </si>
+  <si>
+    <t>Se cambia la clasificaicón del artículo</t>
   </si>
 </sst>
 </file>
@@ -1297,6 +1387,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1309,43 +1408,19 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1357,7 +1432,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1632,7 +1722,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1642,8 +1732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S557"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A459" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H477" sqref="H477:K477"/>
+    <sheetView tabSelected="1" topLeftCell="A484" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D508" sqref="D508"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1652,7 +1742,7 @@
     <col min="2" max="2" width="17.7109375" style="1" customWidth="1"/>
     <col min="3" max="4" width="16.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8" style="52" customWidth="1"/>
+    <col min="6" max="6" width="8" style="60" customWidth="1"/>
     <col min="7" max="7" width="8" style="1" customWidth="1"/>
     <col min="8" max="8" width="4.7109375" style="4" customWidth="1"/>
     <col min="9" max="11" width="16.28515625" style="1" customWidth="1"/>
@@ -1660,32 +1750,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="44" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
       <c r="D1" s="35"/>
-      <c r="E1" s="43"/>
-      <c r="G1" s="48"/>
+      <c r="E1" s="46"/>
+      <c r="G1" s="58"/>
       <c r="H1" s="35" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="35"/>
       <c r="J1" s="35"/>
-      <c r="K1" s="50"/>
+      <c r="K1" s="56"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="42"/>
+      <c r="A2" s="45"/>
       <c r="B2" s="36"/>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
-      <c r="E2" s="44"/>
-      <c r="G2" s="49"/>
+      <c r="E2" s="47"/>
+      <c r="G2" s="59"/>
       <c r="H2" s="36"/>
       <c r="I2" s="36"/>
       <c r="J2" s="36"/>
-      <c r="K2" s="51"/>
+      <c r="K2" s="57"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
@@ -1781,12 +1871,12 @@
       <c r="B9" s="31"/>
       <c r="C9" s="31"/>
       <c r="D9" s="31"/>
-      <c r="H9" s="45" t="s">
+      <c r="H9" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="I9" s="46"/>
-      <c r="J9" s="46"/>
-      <c r="K9" s="47"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="43"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
@@ -1803,18 +1893,18 @@
       <c r="K10" s="30"/>
     </row>
     <row r="11" spans="1:11" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="47"/>
-      <c r="H11" s="45" t="s">
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="43"/>
+      <c r="H11" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="47"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="43"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -2034,32 +2124,32 @@
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="44" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="35"/>
       <c r="C22" s="35"/>
       <c r="D22" s="35"/>
-      <c r="E22" s="43"/>
-      <c r="G22" s="48"/>
+      <c r="E22" s="46"/>
+      <c r="G22" s="58"/>
       <c r="H22" s="35" t="s">
         <v>20</v>
       </c>
       <c r="I22" s="35"/>
       <c r="J22" s="35"/>
-      <c r="K22" s="50"/>
+      <c r="K22" s="56"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="42"/>
+      <c r="A23" s="45"/>
       <c r="B23" s="36"/>
       <c r="C23" s="36"/>
       <c r="D23" s="36"/>
-      <c r="E23" s="44"/>
-      <c r="G23" s="49"/>
+      <c r="E23" s="47"/>
+      <c r="G23" s="59"/>
       <c r="H23" s="36"/>
       <c r="I23" s="36"/>
       <c r="J23" s="36"/>
-      <c r="K23" s="51"/>
+      <c r="K23" s="57"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="37" t="s">
@@ -2151,18 +2241,18 @@
       <c r="K29" s="30"/>
     </row>
     <row r="30" spans="1:11" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="46"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="47"/>
-      <c r="H30" s="45" t="s">
+      <c r="B30" s="42"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="43"/>
+      <c r="H30" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="47"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="43"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="30" t="s">
@@ -2179,18 +2269,18 @@
       <c r="K31" s="30"/>
     </row>
     <row r="32" spans="1:11" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="45" t="s">
+      <c r="A32" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="46"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="47"/>
-      <c r="H32" s="45" t="s">
+      <c r="B32" s="42"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="43"/>
+      <c r="H32" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="47"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="43"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
@@ -2401,32 +2491,32 @@
       <c r="K41" s="31"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="41" t="s">
+      <c r="A43" s="44" t="s">
         <v>21</v>
       </c>
       <c r="B43" s="35"/>
       <c r="C43" s="35"/>
       <c r="D43" s="35"/>
-      <c r="E43" s="43"/>
-      <c r="G43" s="48"/>
+      <c r="E43" s="46"/>
+      <c r="G43" s="58"/>
       <c r="H43" s="35" t="s">
         <v>22</v>
       </c>
       <c r="I43" s="35"/>
       <c r="J43" s="35"/>
-      <c r="K43" s="50"/>
+      <c r="K43" s="56"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="42"/>
+      <c r="A44" s="45"/>
       <c r="B44" s="36"/>
       <c r="C44" s="36"/>
       <c r="D44" s="36"/>
-      <c r="E44" s="44"/>
-      <c r="G44" s="49"/>
+      <c r="E44" s="47"/>
+      <c r="G44" s="59"/>
       <c r="H44" s="36"/>
       <c r="I44" s="36"/>
       <c r="J44" s="36"/>
-      <c r="K44" s="51"/>
+      <c r="K44" s="57"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
@@ -2535,12 +2625,12 @@
       <c r="B51" s="31"/>
       <c r="C51" s="31"/>
       <c r="D51" s="31"/>
-      <c r="H51" s="45" t="s">
+      <c r="H51" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="I51" s="46"/>
-      <c r="J51" s="46"/>
-      <c r="K51" s="47"/>
+      <c r="I51" s="42"/>
+      <c r="J51" s="42"/>
+      <c r="K51" s="43"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="30" t="s">
@@ -2779,32 +2869,32 @@
       <c r="K62" s="31"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="41" t="s">
+      <c r="A64" s="44" t="s">
         <v>25</v>
       </c>
       <c r="B64" s="35"/>
       <c r="C64" s="35"/>
       <c r="D64" s="35"/>
-      <c r="E64" s="43"/>
-      <c r="G64" s="48"/>
+      <c r="E64" s="46"/>
+      <c r="G64" s="58"/>
       <c r="H64" s="35" t="s">
         <v>26</v>
       </c>
       <c r="I64" s="35"/>
       <c r="J64" s="35"/>
-      <c r="K64" s="50"/>
+      <c r="K64" s="56"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="42"/>
+      <c r="A65" s="45"/>
       <c r="B65" s="36"/>
       <c r="C65" s="36"/>
       <c r="D65" s="36"/>
-      <c r="E65" s="44"/>
-      <c r="G65" s="49"/>
+      <c r="E65" s="47"/>
+      <c r="G65" s="59"/>
       <c r="H65" s="36"/>
       <c r="I65" s="36"/>
       <c r="J65" s="36"/>
-      <c r="K65" s="51"/>
+      <c r="K65" s="57"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="37" t="s">
@@ -2901,12 +2991,12 @@
       <c r="B72" s="31"/>
       <c r="C72" s="31"/>
       <c r="D72" s="31"/>
-      <c r="H72" s="45" t="s">
+      <c r="H72" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="I72" s="46"/>
-      <c r="J72" s="46"/>
-      <c r="K72" s="47"/>
+      <c r="I72" s="42"/>
+      <c r="J72" s="42"/>
+      <c r="K72" s="43"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="30" t="s">
@@ -2923,18 +3013,18 @@
       <c r="K73" s="30"/>
     </row>
     <row r="74" spans="1:11" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="45" t="s">
+      <c r="A74" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="B74" s="46"/>
-      <c r="C74" s="46"/>
-      <c r="D74" s="47"/>
-      <c r="H74" s="45" t="s">
+      <c r="B74" s="42"/>
+      <c r="C74" s="42"/>
+      <c r="D74" s="43"/>
+      <c r="H74" s="41" t="s">
         <v>93</v>
       </c>
-      <c r="I74" s="46"/>
-      <c r="J74" s="46"/>
-      <c r="K74" s="47"/>
+      <c r="I74" s="42"/>
+      <c r="J74" s="42"/>
+      <c r="K74" s="43"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
@@ -2979,7 +3069,7 @@
         <v>1</v>
       </c>
       <c r="I76" s="18" t="s">
-        <v>77</v>
+        <v>308</v>
       </c>
       <c r="J76" s="2" t="s">
         <v>38</v>
@@ -2988,7 +3078,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="6">
         <v>2</v>
       </c>
@@ -3005,7 +3095,7 @@
         <v>2</v>
       </c>
       <c r="I77" s="18" t="s">
-        <v>78</v>
+        <v>309</v>
       </c>
       <c r="J77" s="2" t="s">
         <v>38</v>
@@ -3144,32 +3234,32 @@
       <c r="K83" s="31"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A85" s="41" t="s">
+      <c r="A85" s="44" t="s">
         <v>29</v>
       </c>
       <c r="B85" s="35"/>
       <c r="C85" s="35"/>
       <c r="D85" s="35"/>
-      <c r="E85" s="43"/>
-      <c r="G85" s="48"/>
+      <c r="E85" s="46"/>
+      <c r="G85" s="58"/>
       <c r="H85" s="35" t="s">
         <v>31</v>
       </c>
       <c r="I85" s="35"/>
       <c r="J85" s="35"/>
-      <c r="K85" s="50"/>
+      <c r="K85" s="56"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A86" s="42"/>
+      <c r="A86" s="45"/>
       <c r="B86" s="36"/>
       <c r="C86" s="36"/>
       <c r="D86" s="36"/>
-      <c r="E86" s="44"/>
-      <c r="G86" s="49"/>
+      <c r="E86" s="47"/>
+      <c r="G86" s="59"/>
       <c r="H86" s="36"/>
       <c r="I86" s="36"/>
       <c r="J86" s="36"/>
-      <c r="K86" s="51"/>
+      <c r="K86" s="57"/>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="37" t="s">
@@ -3261,12 +3351,12 @@
       <c r="K92" s="30"/>
     </row>
     <row r="93" spans="1:11" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="45" t="s">
+      <c r="A93" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="B93" s="46"/>
-      <c r="C93" s="46"/>
-      <c r="D93" s="47"/>
+      <c r="B93" s="42"/>
+      <c r="C93" s="42"/>
+      <c r="D93" s="43"/>
       <c r="H93" s="31"/>
       <c r="I93" s="31"/>
       <c r="J93" s="31"/>
@@ -3477,32 +3567,32 @@
       <c r="K104" s="31"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A105" s="41" t="s">
+      <c r="A105" s="44" t="s">
         <v>67</v>
       </c>
       <c r="B105" s="35"/>
       <c r="C105" s="35"/>
       <c r="D105" s="35"/>
-      <c r="E105" s="43"/>
-      <c r="G105" s="48"/>
+      <c r="E105" s="46"/>
+      <c r="G105" s="58"/>
       <c r="H105" s="35" t="s">
         <v>82</v>
       </c>
       <c r="I105" s="35"/>
       <c r="J105" s="35"/>
-      <c r="K105" s="50"/>
+      <c r="K105" s="56"/>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A106" s="42"/>
+      <c r="A106" s="45"/>
       <c r="B106" s="36"/>
       <c r="C106" s="36"/>
       <c r="D106" s="36"/>
-      <c r="E106" s="44"/>
-      <c r="G106" s="49"/>
+      <c r="E106" s="47"/>
+      <c r="G106" s="59"/>
       <c r="H106" s="36"/>
       <c r="I106" s="36"/>
       <c r="J106" s="36"/>
-      <c r="K106" s="51"/>
+      <c r="K106" s="57"/>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="37" t="s">
@@ -3598,12 +3688,12 @@
       <c r="B113" s="31"/>
       <c r="C113" s="31"/>
       <c r="D113" s="31"/>
-      <c r="H113" s="45" t="s">
+      <c r="H113" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="I113" s="46"/>
-      <c r="J113" s="46"/>
-      <c r="K113" s="47"/>
+      <c r="I113" s="42"/>
+      <c r="J113" s="42"/>
+      <c r="K113" s="43"/>
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="30" t="s">
@@ -3620,12 +3710,12 @@
       <c r="K114" s="30"/>
     </row>
     <row r="115" spans="1:12" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="45" t="s">
+      <c r="A115" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="B115" s="46"/>
-      <c r="C115" s="46"/>
-      <c r="D115" s="47"/>
+      <c r="B115" s="42"/>
+      <c r="C115" s="42"/>
+      <c r="D115" s="43"/>
       <c r="H115" s="31" t="s">
         <v>108</v>
       </c>
@@ -3848,34 +3938,34 @@
       <c r="E125" s="3"/>
     </row>
     <row r="126" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="41" t="s">
+      <c r="A126" s="44" t="s">
         <v>83</v>
       </c>
       <c r="B126" s="35"/>
       <c r="C126" s="35"/>
       <c r="D126" s="35"/>
-      <c r="E126" s="43"/>
+      <c r="E126" s="46"/>
       <c r="G126" s="20"/>
-      <c r="H126" s="41" t="s">
+      <c r="H126" s="44" t="s">
         <v>84</v>
       </c>
       <c r="I126" s="35"/>
       <c r="J126" s="35"/>
       <c r="K126" s="35"/>
-      <c r="L126" s="43"/>
+      <c r="L126" s="46"/>
     </row>
     <row r="127" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="42"/>
+      <c r="A127" s="45"/>
       <c r="B127" s="36"/>
       <c r="C127" s="36"/>
       <c r="D127" s="36"/>
-      <c r="E127" s="44"/>
+      <c r="E127" s="47"/>
       <c r="G127" s="21"/>
-      <c r="H127" s="42"/>
+      <c r="H127" s="45"/>
       <c r="I127" s="36"/>
       <c r="J127" s="36"/>
       <c r="K127" s="36"/>
-      <c r="L127" s="44"/>
+      <c r="L127" s="47"/>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="37" t="s">
@@ -3976,12 +4066,12 @@
       <c r="B134" s="31"/>
       <c r="C134" s="31"/>
       <c r="D134" s="31"/>
-      <c r="H134" s="45" t="s">
+      <c r="H134" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="I134" s="46"/>
-      <c r="J134" s="46"/>
-      <c r="K134" s="47"/>
+      <c r="I134" s="42"/>
+      <c r="J134" s="42"/>
+      <c r="K134" s="43"/>
     </row>
     <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="30" t="s">
@@ -4220,34 +4310,34 @@
       <c r="L145" s="10"/>
     </row>
     <row r="147" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A147" s="41" t="s">
+      <c r="A147" s="44" t="s">
         <v>85</v>
       </c>
       <c r="B147" s="35"/>
       <c r="C147" s="35"/>
       <c r="D147" s="35"/>
-      <c r="E147" s="43"/>
-      <c r="G147" s="43"/>
-      <c r="H147" s="41" t="s">
+      <c r="E147" s="46"/>
+      <c r="G147" s="46"/>
+      <c r="H147" s="44" t="s">
         <v>86</v>
       </c>
       <c r="I147" s="35"/>
       <c r="J147" s="35"/>
       <c r="K147" s="35"/>
-      <c r="L147" s="43"/>
+      <c r="L147" s="46"/>
     </row>
     <row r="148" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A148" s="42"/>
+      <c r="A148" s="45"/>
       <c r="B148" s="36"/>
       <c r="C148" s="36"/>
       <c r="D148" s="36"/>
-      <c r="E148" s="44"/>
-      <c r="G148" s="44"/>
-      <c r="H148" s="42"/>
+      <c r="E148" s="47"/>
+      <c r="G148" s="47"/>
+      <c r="H148" s="45"/>
       <c r="I148" s="36"/>
       <c r="J148" s="36"/>
       <c r="K148" s="36"/>
-      <c r="L148" s="44"/>
+      <c r="L148" s="47"/>
     </row>
     <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="37" t="s">
@@ -4348,12 +4438,12 @@
       <c r="B155" s="31"/>
       <c r="C155" s="31"/>
       <c r="D155" s="31"/>
-      <c r="H155" s="45" t="s">
+      <c r="H155" s="41" t="s">
         <v>214</v>
       </c>
-      <c r="I155" s="46"/>
-      <c r="J155" s="46"/>
-      <c r="K155" s="47"/>
+      <c r="I155" s="42"/>
+      <c r="J155" s="42"/>
+      <c r="K155" s="43"/>
     </row>
     <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" s="30" t="s">
@@ -4376,12 +4466,12 @@
       <c r="B157" s="31"/>
       <c r="C157" s="31"/>
       <c r="D157" s="31"/>
-      <c r="H157" s="45" t="s">
+      <c r="H157" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="I157" s="46"/>
-      <c r="J157" s="46"/>
-      <c r="K157" s="47"/>
+      <c r="I157" s="42"/>
+      <c r="J157" s="42"/>
+      <c r="K157" s="43"/>
     </row>
     <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" s="13" t="s">
@@ -4594,34 +4684,34 @@
       <c r="L166" s="10"/>
     </row>
     <row r="168" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A168" s="41" t="s">
+      <c r="A168" s="44" t="s">
         <v>87</v>
       </c>
       <c r="B168" s="35"/>
       <c r="C168" s="35"/>
       <c r="D168" s="35"/>
-      <c r="E168" s="43"/>
-      <c r="G168" s="43"/>
-      <c r="H168" s="41" t="s">
+      <c r="E168" s="46"/>
+      <c r="G168" s="46"/>
+      <c r="H168" s="44" t="s">
         <v>88</v>
       </c>
       <c r="I168" s="35"/>
       <c r="J168" s="35"/>
       <c r="K168" s="35"/>
-      <c r="L168" s="43"/>
+      <c r="L168" s="46"/>
     </row>
     <row r="169" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A169" s="42"/>
+      <c r="A169" s="45"/>
       <c r="B169" s="36"/>
       <c r="C169" s="36"/>
       <c r="D169" s="36"/>
-      <c r="E169" s="44"/>
-      <c r="G169" s="44"/>
-      <c r="H169" s="42"/>
+      <c r="E169" s="47"/>
+      <c r="G169" s="47"/>
+      <c r="H169" s="45"/>
       <c r="I169" s="36"/>
       <c r="J169" s="36"/>
       <c r="K169" s="36"/>
-      <c r="L169" s="44"/>
+      <c r="L169" s="47"/>
     </row>
     <row r="171" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A171" s="37" t="s">
@@ -4716,18 +4806,18 @@
       <c r="K175" s="30"/>
     </row>
     <row r="176" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="45" t="s">
+      <c r="A176" s="41" t="s">
         <v>133</v>
       </c>
-      <c r="B176" s="46"/>
-      <c r="C176" s="46"/>
-      <c r="D176" s="47"/>
-      <c r="H176" s="45" t="s">
+      <c r="B176" s="42"/>
+      <c r="C176" s="42"/>
+      <c r="D176" s="43"/>
+      <c r="H176" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="I176" s="46"/>
-      <c r="J176" s="46"/>
-      <c r="K176" s="47"/>
+      <c r="I176" s="42"/>
+      <c r="J176" s="42"/>
+      <c r="K176" s="43"/>
     </row>
     <row r="177" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A177" s="30" t="s">
@@ -4968,14 +5058,14 @@
       <c r="L187" s="10"/>
     </row>
     <row r="189" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A189" s="41" t="s">
+      <c r="A189" s="44" t="s">
         <v>89</v>
       </c>
       <c r="B189" s="35"/>
       <c r="C189" s="35"/>
       <c r="D189" s="35"/>
-      <c r="E189" s="43"/>
-      <c r="F189" s="53"/>
+      <c r="E189" s="46"/>
+      <c r="F189" s="61"/>
       <c r="G189" s="33"/>
       <c r="H189" s="35" t="s">
         <v>90</v>
@@ -4983,21 +5073,21 @@
       <c r="I189" s="35"/>
       <c r="J189" s="35"/>
       <c r="K189" s="35"/>
-      <c r="L189" s="43"/>
+      <c r="L189" s="46"/>
     </row>
     <row r="190" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A190" s="42"/>
+      <c r="A190" s="45"/>
       <c r="B190" s="36"/>
       <c r="C190" s="36"/>
       <c r="D190" s="36"/>
-      <c r="E190" s="44"/>
-      <c r="F190" s="53"/>
+      <c r="E190" s="47"/>
+      <c r="F190" s="61"/>
       <c r="G190" s="34"/>
       <c r="H190" s="36"/>
       <c r="I190" s="36"/>
       <c r="J190" s="36"/>
       <c r="K190" s="36"/>
-      <c r="L190" s="44"/>
+      <c r="L190" s="47"/>
     </row>
     <row r="192" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A192" s="37" t="s">
@@ -5344,14 +5434,14 @@
       <c r="L208" s="10"/>
     </row>
     <row r="210" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A210" s="41" t="s">
+      <c r="A210" s="44" t="s">
         <v>91</v>
       </c>
       <c r="B210" s="35"/>
       <c r="C210" s="35"/>
       <c r="D210" s="35"/>
-      <c r="E210" s="43"/>
-      <c r="F210" s="53"/>
+      <c r="E210" s="46"/>
+      <c r="F210" s="61"/>
       <c r="G210" s="33"/>
       <c r="H210" s="35" t="s">
         <v>92</v>
@@ -5359,21 +5449,21 @@
       <c r="I210" s="35"/>
       <c r="J210" s="35"/>
       <c r="K210" s="35"/>
-      <c r="L210" s="43"/>
+      <c r="L210" s="46"/>
     </row>
     <row r="211" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A211" s="42"/>
+      <c r="A211" s="45"/>
       <c r="B211" s="36"/>
       <c r="C211" s="36"/>
       <c r="D211" s="36"/>
-      <c r="E211" s="44"/>
-      <c r="F211" s="53"/>
+      <c r="E211" s="47"/>
+      <c r="F211" s="61"/>
       <c r="G211" s="34"/>
       <c r="H211" s="36"/>
       <c r="I211" s="36"/>
       <c r="J211" s="36"/>
       <c r="K211" s="36"/>
-      <c r="L211" s="44"/>
+      <c r="L211" s="47"/>
     </row>
     <row r="213" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A213" s="37" t="s">
@@ -5468,18 +5558,18 @@
       <c r="K217" s="30"/>
     </row>
     <row r="218" spans="1:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A218" s="45" t="s">
+      <c r="A218" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="B218" s="46"/>
-      <c r="C218" s="46"/>
-      <c r="D218" s="47"/>
-      <c r="H218" s="45" t="s">
+      <c r="B218" s="42"/>
+      <c r="C218" s="42"/>
+      <c r="D218" s="43"/>
+      <c r="H218" s="41" t="s">
         <v>161</v>
       </c>
-      <c r="I218" s="46"/>
-      <c r="J218" s="46"/>
-      <c r="K218" s="47"/>
+      <c r="I218" s="42"/>
+      <c r="J218" s="42"/>
+      <c r="K218" s="43"/>
     </row>
     <row r="219" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A219" s="30" t="s">
@@ -5720,14 +5810,14 @@
       <c r="L229" s="10"/>
     </row>
     <row r="231" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A231" s="41" t="s">
+      <c r="A231" s="44" t="s">
         <v>105</v>
       </c>
       <c r="B231" s="35"/>
       <c r="C231" s="35"/>
       <c r="D231" s="35"/>
-      <c r="E231" s="43"/>
-      <c r="H231" s="41" t="s">
+      <c r="E231" s="46"/>
+      <c r="H231" s="44" t="s">
         <v>106</v>
       </c>
       <c r="I231" s="35"/>
@@ -5735,12 +5825,12 @@
       <c r="K231" s="35"/>
     </row>
     <row r="232" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A232" s="42"/>
+      <c r="A232" s="45"/>
       <c r="B232" s="36"/>
       <c r="C232" s="36"/>
       <c r="D232" s="36"/>
-      <c r="E232" s="44"/>
-      <c r="H232" s="42"/>
+      <c r="E232" s="47"/>
+      <c r="H232" s="45"/>
       <c r="I232" s="36"/>
       <c r="J232" s="36"/>
       <c r="K232" s="36"/>
@@ -5835,18 +5925,18 @@
       <c r="K238" s="30"/>
     </row>
     <row r="239" spans="1:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="45" t="s">
+      <c r="A239" s="41" t="s">
         <v>176</v>
       </c>
-      <c r="B239" s="46"/>
-      <c r="C239" s="46"/>
-      <c r="D239" s="47"/>
-      <c r="H239" s="45" t="s">
+      <c r="B239" s="42"/>
+      <c r="C239" s="42"/>
+      <c r="D239" s="43"/>
+      <c r="H239" s="41" t="s">
         <v>185</v>
       </c>
-      <c r="I239" s="46"/>
-      <c r="J239" s="46"/>
-      <c r="K239" s="47"/>
+      <c r="I239" s="42"/>
+      <c r="J239" s="42"/>
+      <c r="K239" s="43"/>
     </row>
     <row r="240" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A240" s="30" t="s">
@@ -5863,18 +5953,18 @@
       <c r="K240" s="30"/>
     </row>
     <row r="241" spans="1:16" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A241" s="45" t="s">
+      <c r="A241" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="B241" s="46"/>
-      <c r="C241" s="46"/>
-      <c r="D241" s="47"/>
-      <c r="H241" s="45" t="s">
+      <c r="B241" s="42"/>
+      <c r="C241" s="42"/>
+      <c r="D241" s="43"/>
+      <c r="H241" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="I241" s="46"/>
-      <c r="J241" s="46"/>
-      <c r="K241" s="47"/>
+      <c r="I241" s="42"/>
+      <c r="J241" s="42"/>
+      <c r="K241" s="43"/>
     </row>
     <row r="242" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A242" s="13" t="s">
@@ -6086,14 +6176,14 @@
       <c r="K250" s="31"/>
     </row>
     <row r="253" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A253" s="41" t="s">
+      <c r="A253" s="44" t="s">
         <v>167</v>
       </c>
       <c r="B253" s="35"/>
       <c r="C253" s="35"/>
       <c r="D253" s="35"/>
-      <c r="E253" s="43"/>
-      <c r="F253" s="53"/>
+      <c r="E253" s="46"/>
+      <c r="F253" s="61"/>
       <c r="G253" s="33"/>
       <c r="H253" s="35" t="s">
         <v>168</v>
@@ -6103,12 +6193,12 @@
       <c r="K253" s="35"/>
     </row>
     <row r="254" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A254" s="42"/>
+      <c r="A254" s="45"/>
       <c r="B254" s="36"/>
       <c r="C254" s="36"/>
       <c r="D254" s="36"/>
-      <c r="E254" s="44"/>
-      <c r="F254" s="53"/>
+      <c r="E254" s="47"/>
+      <c r="F254" s="61"/>
       <c r="G254" s="34"/>
       <c r="H254" s="36"/>
       <c r="I254" s="36"/>
@@ -6205,18 +6295,18 @@
       <c r="K260" s="30"/>
     </row>
     <row r="261" spans="1:11" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A261" s="45" t="s">
+      <c r="A261" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="B261" s="46"/>
-      <c r="C261" s="46"/>
-      <c r="D261" s="47"/>
-      <c r="H261" s="45" t="s">
+      <c r="B261" s="42"/>
+      <c r="C261" s="42"/>
+      <c r="D261" s="43"/>
+      <c r="H261" s="41" t="s">
         <v>192</v>
       </c>
-      <c r="I261" s="46"/>
-      <c r="J261" s="46"/>
-      <c r="K261" s="47"/>
+      <c r="I261" s="42"/>
+      <c r="J261" s="42"/>
+      <c r="K261" s="43"/>
     </row>
     <row r="262" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A262" s="30" t="s">
@@ -6233,18 +6323,18 @@
       <c r="K262" s="30"/>
     </row>
     <row r="263" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A263" s="45" t="s">
+      <c r="A263" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="B263" s="46"/>
-      <c r="C263" s="46"/>
-      <c r="D263" s="47"/>
-      <c r="H263" s="45" t="s">
+      <c r="B263" s="42"/>
+      <c r="C263" s="42"/>
+      <c r="D263" s="43"/>
+      <c r="H263" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="I263" s="46"/>
-      <c r="J263" s="46"/>
-      <c r="K263" s="47"/>
+      <c r="I263" s="42"/>
+      <c r="J263" s="42"/>
+      <c r="K263" s="43"/>
     </row>
     <row r="264" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A264" s="17" t="s">
@@ -6455,14 +6545,14 @@
       <c r="K272" s="31"/>
     </row>
     <row r="274" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A274" s="41" t="s">
+      <c r="A274" s="44" t="s">
         <v>169</v>
       </c>
       <c r="B274" s="35"/>
       <c r="C274" s="35"/>
       <c r="D274" s="35"/>
-      <c r="E274" s="43"/>
-      <c r="F274" s="53"/>
+      <c r="E274" s="46"/>
+      <c r="F274" s="61"/>
       <c r="G274" s="33"/>
       <c r="H274" s="35" t="s">
         <v>170</v>
@@ -6472,12 +6562,12 @@
       <c r="K274" s="35"/>
     </row>
     <row r="275" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A275" s="42"/>
+      <c r="A275" s="45"/>
       <c r="B275" s="36"/>
       <c r="C275" s="36"/>
       <c r="D275" s="36"/>
-      <c r="E275" s="44"/>
-      <c r="F275" s="53"/>
+      <c r="E275" s="47"/>
+      <c r="F275" s="61"/>
       <c r="G275" s="34"/>
       <c r="H275" s="36"/>
       <c r="I275" s="36"/>
@@ -6580,12 +6670,12 @@
       <c r="B282" s="31"/>
       <c r="C282" s="31"/>
       <c r="D282" s="31"/>
-      <c r="H282" s="45" t="s">
+      <c r="H282" s="41" t="s">
         <v>204</v>
       </c>
-      <c r="I282" s="46"/>
-      <c r="J282" s="46"/>
-      <c r="K282" s="47"/>
+      <c r="I282" s="42"/>
+      <c r="J282" s="42"/>
+      <c r="K282" s="43"/>
     </row>
     <row r="283" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A283" s="30" t="s">
@@ -6602,18 +6692,18 @@
       <c r="K283" s="30"/>
     </row>
     <row r="284" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A284" s="45" t="s">
+      <c r="A284" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="B284" s="46"/>
-      <c r="C284" s="46"/>
-      <c r="D284" s="47"/>
-      <c r="H284" s="45" t="s">
+      <c r="B284" s="42"/>
+      <c r="C284" s="42"/>
+      <c r="D284" s="43"/>
+      <c r="H284" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="I284" s="46"/>
-      <c r="J284" s="46"/>
-      <c r="K284" s="47"/>
+      <c r="I284" s="42"/>
+      <c r="J284" s="42"/>
+      <c r="K284" s="43"/>
     </row>
     <row r="285" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A285" s="17" t="s">
@@ -6825,13 +6915,13 @@
       <c r="K293" s="31"/>
     </row>
     <row r="295" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A295" s="41" t="s">
+      <c r="A295" s="44" t="s">
         <v>171</v>
       </c>
       <c r="B295" s="35"/>
       <c r="C295" s="35"/>
       <c r="D295" s="35"/>
-      <c r="E295" s="43"/>
+      <c r="E295" s="46"/>
       <c r="G295" s="33"/>
       <c r="H295" s="35" t="s">
         <v>172</v>
@@ -6841,11 +6931,11 @@
       <c r="K295" s="35"/>
     </row>
     <row r="296" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A296" s="42"/>
+      <c r="A296" s="45"/>
       <c r="B296" s="36"/>
       <c r="C296" s="36"/>
       <c r="D296" s="36"/>
-      <c r="E296" s="44"/>
+      <c r="E296" s="47"/>
       <c r="G296" s="34"/>
       <c r="H296" s="36"/>
       <c r="I296" s="36"/>
@@ -6942,18 +7032,18 @@
       <c r="K302" s="30"/>
     </row>
     <row r="303" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A303" s="45" t="s">
+      <c r="A303" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="B303" s="46"/>
-      <c r="C303" s="46"/>
-      <c r="D303" s="47"/>
-      <c r="H303" s="45" t="s">
+      <c r="B303" s="42"/>
+      <c r="C303" s="42"/>
+      <c r="D303" s="43"/>
+      <c r="H303" s="41" t="s">
         <v>217</v>
       </c>
-      <c r="I303" s="46"/>
-      <c r="J303" s="46"/>
-      <c r="K303" s="47"/>
+      <c r="I303" s="42"/>
+      <c r="J303" s="42"/>
+      <c r="K303" s="43"/>
     </row>
     <row r="304" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A304" s="30" t="s">
@@ -6976,12 +7066,12 @@
       <c r="B305" s="31"/>
       <c r="C305" s="31"/>
       <c r="D305" s="31"/>
-      <c r="H305" s="45" t="s">
+      <c r="H305" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="I305" s="46"/>
-      <c r="J305" s="46"/>
-      <c r="K305" s="47"/>
+      <c r="I305" s="42"/>
+      <c r="J305" s="42"/>
+      <c r="K305" s="43"/>
     </row>
     <row r="306" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A306" s="17" t="s">
@@ -7140,12 +7230,12 @@
       </c>
     </row>
     <row r="312" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A312" s="58" t="s">
+      <c r="A312" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="B312" s="59"/>
-      <c r="C312" s="59"/>
-      <c r="D312" s="60"/>
+      <c r="B312" s="54"/>
+      <c r="C312" s="54"/>
+      <c r="D312" s="55"/>
       <c r="H312" s="30" t="s">
         <v>10</v>
       </c>
@@ -7192,13 +7282,13 @@
       <c r="K314" s="31"/>
     </row>
     <row r="316" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A316" s="41" t="s">
+      <c r="A316" s="44" t="s">
         <v>173</v>
       </c>
       <c r="B316" s="35"/>
       <c r="C316" s="35"/>
       <c r="D316" s="35"/>
-      <c r="E316" s="43"/>
+      <c r="E316" s="46"/>
       <c r="G316" s="33"/>
       <c r="H316" s="35" t="s">
         <v>174</v>
@@ -7208,11 +7298,11 @@
       <c r="K316" s="35"/>
     </row>
     <row r="317" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A317" s="42"/>
+      <c r="A317" s="45"/>
       <c r="B317" s="36"/>
       <c r="C317" s="36"/>
       <c r="D317" s="36"/>
-      <c r="E317" s="44"/>
+      <c r="E317" s="47"/>
       <c r="G317" s="34"/>
       <c r="H317" s="36"/>
       <c r="I317" s="36"/>
@@ -7295,12 +7385,12 @@
       <c r="K322" s="40"/>
     </row>
     <row r="323" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A323" s="61" t="s">
+      <c r="A323" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B323" s="61"/>
-      <c r="C323" s="61"/>
-      <c r="D323" s="61"/>
+      <c r="B323" s="50"/>
+      <c r="C323" s="50"/>
+      <c r="D323" s="50"/>
       <c r="H323" s="30" t="s">
         <v>5</v>
       </c>
@@ -7309,26 +7399,26 @@
       <c r="K323" s="30"/>
     </row>
     <row r="324" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A324" s="56" t="s">
+      <c r="A324" s="48" t="s">
         <v>225</v>
       </c>
-      <c r="B324" s="56"/>
-      <c r="C324" s="56"/>
-      <c r="D324" s="57"/>
-      <c r="H324" s="45" t="s">
+      <c r="B324" s="48"/>
+      <c r="C324" s="48"/>
+      <c r="D324" s="49"/>
+      <c r="H324" s="41" t="s">
         <v>241</v>
       </c>
-      <c r="I324" s="46"/>
-      <c r="J324" s="46"/>
-      <c r="K324" s="47"/>
+      <c r="I324" s="42"/>
+      <c r="J324" s="42"/>
+      <c r="K324" s="43"/>
     </row>
     <row r="325" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A325" s="54" t="s">
+      <c r="A325" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="B325" s="54"/>
-      <c r="C325" s="54"/>
-      <c r="D325" s="54"/>
+      <c r="B325" s="51"/>
+      <c r="C325" s="51"/>
+      <c r="D325" s="51"/>
       <c r="H325" s="30" t="s">
         <v>2</v>
       </c>
@@ -7337,18 +7427,18 @@
       <c r="K325" s="30"/>
     </row>
     <row r="326" spans="1:11" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A326" s="55" t="s">
+      <c r="A326" s="52" t="s">
         <v>226</v>
       </c>
-      <c r="B326" s="56"/>
-      <c r="C326" s="56"/>
-      <c r="D326" s="57"/>
-      <c r="H326" s="45" t="s">
+      <c r="B326" s="48"/>
+      <c r="C326" s="48"/>
+      <c r="D326" s="49"/>
+      <c r="H326" s="41" t="s">
         <v>242</v>
       </c>
-      <c r="I326" s="46"/>
-      <c r="J326" s="46"/>
-      <c r="K326" s="47"/>
+      <c r="I326" s="42"/>
+      <c r="J326" s="42"/>
+      <c r="K326" s="43"/>
     </row>
     <row r="327" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A327" s="17" t="s">
@@ -7557,13 +7647,13 @@
       <c r="K335" s="31"/>
     </row>
     <row r="338" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A338" s="41" t="s">
+      <c r="A338" s="44" t="s">
         <v>223</v>
       </c>
       <c r="B338" s="35"/>
       <c r="C338" s="35"/>
       <c r="D338" s="35"/>
-      <c r="E338" s="43"/>
+      <c r="E338" s="46"/>
       <c r="G338" s="33"/>
       <c r="H338" s="35" t="s">
         <v>224</v>
@@ -7573,11 +7663,11 @@
       <c r="K338" s="35"/>
     </row>
     <row r="339" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A339" s="42"/>
+      <c r="A339" s="45"/>
       <c r="B339" s="36"/>
       <c r="C339" s="36"/>
       <c r="D339" s="36"/>
-      <c r="E339" s="44"/>
+      <c r="E339" s="47"/>
       <c r="G339" s="34"/>
       <c r="H339" s="36"/>
       <c r="I339" s="36"/>
@@ -7674,18 +7764,18 @@
       <c r="K345" s="30"/>
     </row>
     <row r="346" spans="1:19" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A346" s="45" t="s">
+      <c r="A346" s="41" t="s">
         <v>241</v>
       </c>
-      <c r="B346" s="46"/>
-      <c r="C346" s="46"/>
-      <c r="D346" s="47"/>
-      <c r="H346" s="45" t="s">
+      <c r="B346" s="42"/>
+      <c r="C346" s="42"/>
+      <c r="D346" s="43"/>
+      <c r="H346" s="41" t="s">
         <v>249</v>
       </c>
-      <c r="I346" s="46"/>
-      <c r="J346" s="46"/>
-      <c r="K346" s="47"/>
+      <c r="I346" s="42"/>
+      <c r="J346" s="42"/>
+      <c r="K346" s="43"/>
     </row>
     <row r="347" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A347" s="30" t="s">
@@ -7702,18 +7792,18 @@
       <c r="K347" s="30"/>
     </row>
     <row r="348" spans="1:19" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A348" s="45" t="s">
+      <c r="A348" s="41" t="s">
         <v>242</v>
       </c>
-      <c r="B348" s="46"/>
-      <c r="C348" s="46"/>
-      <c r="D348" s="47"/>
-      <c r="H348" s="45" t="s">
+      <c r="B348" s="42"/>
+      <c r="C348" s="42"/>
+      <c r="D348" s="43"/>
+      <c r="H348" s="41" t="s">
         <v>250</v>
       </c>
-      <c r="I348" s="46"/>
-      <c r="J348" s="46"/>
-      <c r="K348" s="47"/>
+      <c r="I348" s="42"/>
+      <c r="J348" s="42"/>
+      <c r="K348" s="43"/>
       <c r="S348" s="23"/>
     </row>
     <row r="349" spans="1:19" x14ac:dyDescent="0.25">
@@ -7925,13 +8015,13 @@
       <c r="K357" s="31"/>
     </row>
     <row r="360" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A360" s="41" t="s">
+      <c r="A360" s="44" t="s">
         <v>232</v>
       </c>
       <c r="B360" s="35"/>
       <c r="C360" s="35"/>
       <c r="D360" s="35"/>
-      <c r="E360" s="43"/>
+      <c r="E360" s="46"/>
       <c r="G360" s="33"/>
       <c r="H360" s="35" t="s">
         <v>233</v>
@@ -7941,11 +8031,11 @@
       <c r="K360" s="35"/>
     </row>
     <row r="361" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A361" s="42"/>
+      <c r="A361" s="45"/>
       <c r="B361" s="36"/>
       <c r="C361" s="36"/>
       <c r="D361" s="36"/>
-      <c r="E361" s="44"/>
+      <c r="E361" s="47"/>
       <c r="G361" s="34"/>
       <c r="H361" s="36"/>
       <c r="I361" s="36"/>
@@ -8042,18 +8132,18 @@
       <c r="K367" s="30"/>
     </row>
     <row r="368" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A368" s="45" t="s">
+      <c r="A368" s="41" t="s">
         <v>249</v>
       </c>
-      <c r="B368" s="46"/>
-      <c r="C368" s="46"/>
-      <c r="D368" s="47"/>
-      <c r="H368" s="45" t="s">
+      <c r="B368" s="42"/>
+      <c r="C368" s="42"/>
+      <c r="D368" s="43"/>
+      <c r="H368" s="41" t="s">
         <v>264</v>
       </c>
-      <c r="I368" s="46"/>
-      <c r="J368" s="46"/>
-      <c r="K368" s="47"/>
+      <c r="I368" s="42"/>
+      <c r="J368" s="42"/>
+      <c r="K368" s="43"/>
     </row>
     <row r="369" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A369" s="30" t="s">
@@ -8070,18 +8160,18 @@
       <c r="K369" s="30"/>
     </row>
     <row r="370" spans="1:11" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A370" s="45" t="s">
+      <c r="A370" s="41" t="s">
         <v>250</v>
       </c>
-      <c r="B370" s="46"/>
-      <c r="C370" s="46"/>
-      <c r="D370" s="47"/>
-      <c r="H370" s="45" t="s">
+      <c r="B370" s="42"/>
+      <c r="C370" s="42"/>
+      <c r="D370" s="43"/>
+      <c r="H370" s="41" t="s">
         <v>265</v>
       </c>
-      <c r="I370" s="46"/>
-      <c r="J370" s="46"/>
-      <c r="K370" s="47"/>
+      <c r="I370" s="42"/>
+      <c r="J370" s="42"/>
+      <c r="K370" s="43"/>
     </row>
     <row r="371" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A371" s="26" t="s">
@@ -8292,13 +8382,13 @@
       <c r="K379" s="31"/>
     </row>
     <row r="381" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A381" s="41" t="s">
+      <c r="A381" s="44" t="s">
         <v>234</v>
       </c>
       <c r="B381" s="35"/>
       <c r="C381" s="35"/>
       <c r="D381" s="35"/>
-      <c r="E381" s="43"/>
+      <c r="E381" s="46"/>
       <c r="G381" s="33"/>
       <c r="H381" s="35" t="s">
         <v>235</v>
@@ -8308,11 +8398,11 @@
       <c r="K381" s="35"/>
     </row>
     <row r="382" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A382" s="42"/>
+      <c r="A382" s="45"/>
       <c r="B382" s="36"/>
       <c r="C382" s="36"/>
       <c r="D382" s="36"/>
-      <c r="E382" s="44"/>
+      <c r="E382" s="47"/>
       <c r="G382" s="34"/>
       <c r="H382" s="36"/>
       <c r="I382" s="36"/>
@@ -8435,12 +8525,12 @@
       <c r="K390" s="30"/>
     </row>
     <row r="391" spans="1:11" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A391" s="45" t="s">
+      <c r="A391" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="B391" s="46"/>
-      <c r="C391" s="46"/>
-      <c r="D391" s="47"/>
+      <c r="B391" s="42"/>
+      <c r="C391" s="42"/>
+      <c r="D391" s="43"/>
       <c r="H391" s="31"/>
       <c r="I391" s="31"/>
       <c r="J391" s="31"/>
@@ -8625,13 +8715,13 @@
       <c r="K400" s="31"/>
     </row>
     <row r="403" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A403" s="41" t="s">
+      <c r="A403" s="44" t="s">
         <v>261</v>
       </c>
       <c r="B403" s="35"/>
       <c r="C403" s="35"/>
       <c r="D403" s="35"/>
-      <c r="E403" s="43"/>
+      <c r="E403" s="46"/>
       <c r="G403" s="33"/>
       <c r="H403" s="35" t="s">
         <v>262</v>
@@ -8641,11 +8731,11 @@
       <c r="K403" s="35"/>
     </row>
     <row r="404" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A404" s="42"/>
+      <c r="A404" s="45"/>
       <c r="B404" s="36"/>
       <c r="C404" s="36"/>
       <c r="D404" s="36"/>
-      <c r="E404" s="44"/>
+      <c r="E404" s="47"/>
       <c r="G404" s="34"/>
       <c r="H404" s="36"/>
       <c r="I404" s="36"/>
@@ -8740,12 +8830,12 @@
       <c r="K410" s="30"/>
     </row>
     <row r="411" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A411" s="45" t="s">
+      <c r="A411" s="41" t="s">
         <v>279</v>
       </c>
-      <c r="B411" s="46"/>
-      <c r="C411" s="46"/>
-      <c r="D411" s="47"/>
+      <c r="B411" s="42"/>
+      <c r="C411" s="42"/>
+      <c r="D411" s="43"/>
       <c r="H411" s="31"/>
       <c r="I411" s="31"/>
       <c r="J411" s="31"/>
@@ -8926,13 +9016,13 @@
       <c r="K422" s="31"/>
     </row>
     <row r="425" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A425" s="41" t="s">
+      <c r="A425" s="44" t="s">
         <v>261</v>
       </c>
       <c r="B425" s="35"/>
       <c r="C425" s="35"/>
       <c r="D425" s="35"/>
-      <c r="E425" s="43"/>
+      <c r="E425" s="46"/>
       <c r="G425" s="33"/>
       <c r="H425" s="35" t="s">
         <v>262</v>
@@ -8942,11 +9032,11 @@
       <c r="K425" s="35"/>
     </row>
     <row r="426" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A426" s="42"/>
+      <c r="A426" s="45"/>
       <c r="B426" s="36"/>
       <c r="C426" s="36"/>
       <c r="D426" s="36"/>
-      <c r="E426" s="44"/>
+      <c r="E426" s="47"/>
       <c r="G426" s="34"/>
       <c r="H426" s="36"/>
       <c r="I426" s="36"/>
@@ -9043,18 +9133,18 @@
       <c r="K432" s="30"/>
     </row>
     <row r="433" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A433" s="45" t="s">
+      <c r="A433" s="41" t="s">
         <v>279</v>
       </c>
-      <c r="B433" s="46"/>
-      <c r="C433" s="46"/>
-      <c r="D433" s="47"/>
-      <c r="H433" s="45" t="s">
+      <c r="B433" s="42"/>
+      <c r="C433" s="42"/>
+      <c r="D433" s="43"/>
+      <c r="H433" s="41" t="s">
         <v>289</v>
       </c>
-      <c r="I433" s="46"/>
-      <c r="J433" s="46"/>
-      <c r="K433" s="47"/>
+      <c r="I433" s="42"/>
+      <c r="J433" s="42"/>
+      <c r="K433" s="43"/>
     </row>
     <row r="434" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A434" s="30" t="s">
@@ -9071,18 +9161,18 @@
       <c r="K434" s="30"/>
     </row>
     <row r="435" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A435" s="45" t="s">
+      <c r="A435" s="41" t="s">
         <v>280</v>
       </c>
-      <c r="B435" s="46"/>
-      <c r="C435" s="46"/>
-      <c r="D435" s="47"/>
-      <c r="H435" s="45" t="s">
+      <c r="B435" s="42"/>
+      <c r="C435" s="42"/>
+      <c r="D435" s="43"/>
+      <c r="H435" s="41" t="s">
         <v>291</v>
       </c>
-      <c r="I435" s="46"/>
-      <c r="J435" s="46"/>
-      <c r="K435" s="47"/>
+      <c r="I435" s="42"/>
+      <c r="J435" s="42"/>
+      <c r="K435" s="43"/>
     </row>
     <row r="436" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A436" s="28" t="s">
@@ -9293,13 +9383,13 @@
       <c r="K444" s="31"/>
     </row>
     <row r="447" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A447" s="41" t="s">
+      <c r="A447" s="44" t="s">
         <v>282</v>
       </c>
       <c r="B447" s="35"/>
       <c r="C447" s="35"/>
       <c r="D447" s="35"/>
-      <c r="E447" s="43"/>
+      <c r="E447" s="46"/>
       <c r="G447" s="33"/>
       <c r="H447" s="35" t="s">
         <v>283</v>
@@ -9309,11 +9399,11 @@
       <c r="K447" s="35"/>
     </row>
     <row r="448" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A448" s="42"/>
+      <c r="A448" s="45"/>
       <c r="B448" s="36"/>
       <c r="C448" s="36"/>
       <c r="D448" s="36"/>
-      <c r="E448" s="44"/>
+      <c r="E448" s="47"/>
       <c r="G448" s="34"/>
       <c r="H448" s="36"/>
       <c r="I448" s="36"/>
@@ -9410,12 +9500,12 @@
       <c r="K454" s="30"/>
     </row>
     <row r="455" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H455" s="45" t="s">
+      <c r="H455" s="41" t="s">
         <v>304</v>
       </c>
-      <c r="I455" s="46"/>
-      <c r="J455" s="46"/>
-      <c r="K455" s="47"/>
+      <c r="I455" s="42"/>
+      <c r="J455" s="42"/>
+      <c r="K455" s="43"/>
     </row>
     <row r="456" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A456" s="30" t="s">
@@ -9432,12 +9522,12 @@
       <c r="K456" s="30"/>
     </row>
     <row r="457" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H457" s="45" t="s">
+      <c r="H457" s="41" t="s">
         <v>305</v>
       </c>
-      <c r="I457" s="46"/>
-      <c r="J457" s="46"/>
-      <c r="K457" s="47"/>
+      <c r="I457" s="42"/>
+      <c r="J457" s="42"/>
+      <c r="K457" s="43"/>
     </row>
     <row r="458" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A458" s="28" t="s">
@@ -9618,13 +9708,13 @@
       <c r="K466" s="31"/>
     </row>
     <row r="469" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A469" s="41" t="s">
+      <c r="A469" s="44" t="s">
         <v>294</v>
       </c>
       <c r="B469" s="35"/>
       <c r="C469" s="35"/>
       <c r="D469" s="35"/>
-      <c r="E469" s="43"/>
+      <c r="E469" s="46"/>
       <c r="G469" s="33"/>
       <c r="H469" s="35" t="s">
         <v>295</v>
@@ -9634,11 +9724,11 @@
       <c r="K469" s="35"/>
     </row>
     <row r="470" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A470" s="42"/>
+      <c r="A470" s="45"/>
       <c r="B470" s="36"/>
       <c r="C470" s="36"/>
       <c r="D470" s="36"/>
-      <c r="E470" s="44"/>
+      <c r="E470" s="47"/>
       <c r="G470" s="34"/>
       <c r="H470" s="36"/>
       <c r="I470" s="36"/>
@@ -9689,7 +9779,7 @@
       </c>
       <c r="B474" s="38"/>
       <c r="C474" s="39" t="s">
-        <v>259</v>
+        <v>321</v>
       </c>
       <c r="D474" s="40"/>
       <c r="E474" s="9"/>
@@ -9698,7 +9788,7 @@
       </c>
       <c r="I474" s="38"/>
       <c r="J474" s="39" t="s">
-        <v>260</v>
+        <v>320</v>
       </c>
       <c r="K474" s="40"/>
     </row>
@@ -9708,7 +9798,7 @@
       </c>
       <c r="B475" s="38"/>
       <c r="C475" s="39" t="s">
-        <v>281</v>
+        <v>316</v>
       </c>
       <c r="D475" s="40"/>
       <c r="H475" s="37" t="s">
@@ -9716,7 +9806,7 @@
       </c>
       <c r="I475" s="38"/>
       <c r="J475" s="39" t="s">
-        <v>281</v>
+        <v>322</v>
       </c>
       <c r="K475" s="40"/>
     </row>
@@ -9735,14 +9825,18 @@
       <c r="K476" s="30"/>
     </row>
     <row r="477" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A477" s="45"/>
-      <c r="B477" s="46"/>
-      <c r="C477" s="46"/>
-      <c r="D477" s="47"/>
-      <c r="H477" s="45"/>
-      <c r="I477" s="46"/>
-      <c r="J477" s="46"/>
-      <c r="K477" s="47"/>
+      <c r="A477" s="41" t="s">
+        <v>313</v>
+      </c>
+      <c r="B477" s="42"/>
+      <c r="C477" s="42"/>
+      <c r="D477" s="43"/>
+      <c r="H477" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="I477" s="42"/>
+      <c r="J477" s="42"/>
+      <c r="K477" s="43"/>
     </row>
     <row r="478" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A478" s="30" t="s">
@@ -9758,15 +9852,19 @@
       <c r="J478" s="30"/>
       <c r="K478" s="30"/>
     </row>
-    <row r="479" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A479" s="31"/>
-      <c r="B479" s="31"/>
-      <c r="C479" s="31"/>
-      <c r="D479" s="31"/>
-      <c r="H479" s="31"/>
-      <c r="I479" s="31"/>
-      <c r="J479" s="31"/>
-      <c r="K479" s="31"/>
+    <row r="479" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A479" s="41" t="s">
+        <v>312</v>
+      </c>
+      <c r="B479" s="42"/>
+      <c r="C479" s="42"/>
+      <c r="D479" s="43"/>
+      <c r="H479" s="41" t="s">
+        <v>318</v>
+      </c>
+      <c r="I479" s="42"/>
+      <c r="J479" s="42"/>
+      <c r="K479" s="43"/>
     </row>
     <row r="480" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A480" s="28" t="s">
@@ -9794,75 +9892,135 @@
         <v>16</v>
       </c>
     </row>
-    <row r="481" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A481" s="29">
         <v>1</v>
       </c>
-      <c r="B481" s="2"/>
-      <c r="C481" s="2"/>
-      <c r="D481" s="2"/>
+      <c r="B481" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="C481" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D481" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="H481" s="29">
         <v>1</v>
       </c>
-      <c r="I481" s="2"/>
-      <c r="J481" s="2"/>
-      <c r="K481" s="2"/>
-    </row>
-    <row r="482" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I481" s="18" t="s">
+        <v>323</v>
+      </c>
+      <c r="J481" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K481" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="482" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A482" s="29">
         <v>2</v>
       </c>
-      <c r="B482" s="2"/>
-      <c r="C482" s="2"/>
-      <c r="D482" s="2"/>
+      <c r="B482" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="C482" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D482" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="H482" s="29">
         <v>2</v>
       </c>
-      <c r="I482" s="2"/>
-      <c r="J482" s="2"/>
-      <c r="K482" s="2"/>
-    </row>
-    <row r="483" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I482" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="J482" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K482" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="483" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A483" s="29">
         <v>3</v>
       </c>
-      <c r="B483" s="2"/>
-      <c r="C483" s="2"/>
-      <c r="D483" s="2"/>
+      <c r="B483" s="18" t="s">
+        <v>314</v>
+      </c>
+      <c r="C483" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D483" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="H483" s="29">
         <v>3</v>
       </c>
-      <c r="I483" s="2"/>
-      <c r="J483" s="2"/>
-      <c r="K483" s="2"/>
-    </row>
-    <row r="484" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I483" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="J483" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="K483" s="18" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="484" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A484" s="29">
         <v>4</v>
       </c>
-      <c r="B484" s="2"/>
-      <c r="C484" s="2"/>
-      <c r="D484" s="2"/>
+      <c r="B484" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="C484" s="18" t="s">
+        <v>317</v>
+      </c>
+      <c r="D484" s="18" t="s">
+        <v>317</v>
+      </c>
       <c r="H484" s="29">
         <v>4</v>
       </c>
-      <c r="I484" s="2"/>
-      <c r="J484" s="2"/>
-      <c r="K484" s="2"/>
+      <c r="I484" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="J484" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="K484" s="18" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="485" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A485" s="29">
         <v>5</v>
       </c>
-      <c r="B485" s="2"/>
-      <c r="C485" s="2"/>
-      <c r="D485" s="2"/>
+      <c r="B485" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C485" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D485" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="H485" s="29">
         <v>5</v>
       </c>
-      <c r="I485" s="2"/>
-      <c r="J485" s="2"/>
-      <c r="K485" s="2"/>
+      <c r="I485" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J485" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K485" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="486" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A486" s="30" t="s">
@@ -9917,13 +10075,13 @@
       <c r="K488" s="31"/>
     </row>
     <row r="492" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A492" s="41" t="s">
+      <c r="A492" s="44" t="s">
         <v>296</v>
       </c>
       <c r="B492" s="35"/>
       <c r="C492" s="35"/>
       <c r="D492" s="35"/>
-      <c r="E492" s="43"/>
+      <c r="E492" s="46"/>
       <c r="G492" s="33"/>
       <c r="H492" s="35" t="s">
         <v>297</v>
@@ -9933,11 +10091,11 @@
       <c r="K492" s="35"/>
     </row>
     <row r="493" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A493" s="42"/>
+      <c r="A493" s="45"/>
       <c r="B493" s="36"/>
       <c r="C493" s="36"/>
       <c r="D493" s="36"/>
-      <c r="E493" s="44"/>
+      <c r="E493" s="47"/>
       <c r="G493" s="34"/>
       <c r="H493" s="36"/>
       <c r="I493" s="36"/>
@@ -9988,7 +10146,7 @@
       </c>
       <c r="B497" s="38"/>
       <c r="C497" s="39" t="s">
-        <v>259</v>
+        <v>329</v>
       </c>
       <c r="D497" s="40"/>
       <c r="E497" s="9"/>
@@ -9997,7 +10155,7 @@
       </c>
       <c r="I497" s="38"/>
       <c r="J497" s="39" t="s">
-        <v>260</v>
+        <v>330</v>
       </c>
       <c r="K497" s="40"/>
     </row>
@@ -10033,11 +10191,13 @@
       <c r="J499" s="30"/>
       <c r="K499" s="30"/>
     </row>
-    <row r="500" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A500" s="45"/>
-      <c r="B500" s="46"/>
-      <c r="C500" s="46"/>
-      <c r="D500" s="47"/>
+    <row r="500" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A500" s="41" t="s">
+        <v>331</v>
+      </c>
+      <c r="B500" s="42"/>
+      <c r="C500" s="42"/>
+      <c r="D500" s="43"/>
       <c r="H500" s="31"/>
       <c r="I500" s="31"/>
       <c r="J500" s="31"/>
@@ -10057,11 +10217,13 @@
       <c r="J501" s="30"/>
       <c r="K501" s="30"/>
     </row>
-    <row r="502" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A502" s="31"/>
-      <c r="B502" s="31"/>
-      <c r="C502" s="31"/>
-      <c r="D502" s="31"/>
+    <row r="502" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A502" s="41" t="s">
+        <v>332</v>
+      </c>
+      <c r="B502" s="42"/>
+      <c r="C502" s="42"/>
+      <c r="D502" s="43"/>
       <c r="H502" s="31"/>
       <c r="I502" s="31"/>
       <c r="J502" s="31"/>
@@ -10093,13 +10255,19 @@
         <v>16</v>
       </c>
     </row>
-    <row r="504" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A504" s="29">
         <v>1</v>
       </c>
-      <c r="B504" s="2"/>
-      <c r="C504" s="2"/>
-      <c r="D504" s="2"/>
+      <c r="B504" s="18" t="s">
+        <v>333</v>
+      </c>
+      <c r="C504" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="D504" s="18" t="s">
+        <v>334</v>
+      </c>
       <c r="H504" s="29">
         <v>1</v>
       </c>
@@ -10107,13 +10275,19 @@
       <c r="J504" s="2"/>
       <c r="K504" s="2"/>
     </row>
-    <row r="505" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A505" s="29">
         <v>2</v>
       </c>
-      <c r="B505" s="2"/>
-      <c r="C505" s="2"/>
-      <c r="D505" s="2"/>
+      <c r="B505" s="18" t="s">
+        <v>335</v>
+      </c>
+      <c r="C505" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D505" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="H505" s="29">
         <v>2</v>
       </c>
@@ -10121,13 +10295,19 @@
       <c r="J505" s="2"/>
       <c r="K505" s="2"/>
     </row>
-    <row r="506" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A506" s="29">
         <v>3</v>
       </c>
-      <c r="B506" s="2"/>
-      <c r="C506" s="2"/>
-      <c r="D506" s="2"/>
+      <c r="B506" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="C506" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="D506" s="18" t="s">
+        <v>337</v>
+      </c>
       <c r="H506" s="29">
         <v>3</v>
       </c>
@@ -10139,9 +10319,15 @@
       <c r="A507" s="29">
         <v>4</v>
       </c>
-      <c r="B507" s="2"/>
-      <c r="C507" s="2"/>
-      <c r="D507" s="2"/>
+      <c r="B507" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C507" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D507" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="H507" s="29">
         <v>4</v>
       </c>
@@ -10153,9 +10339,15 @@
       <c r="A508" s="29">
         <v>5</v>
       </c>
-      <c r="B508" s="2"/>
-      <c r="C508" s="2"/>
-      <c r="D508" s="2"/>
+      <c r="B508" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C508" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D508" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="H508" s="29">
         <v>5</v>
       </c>
@@ -10216,13 +10408,13 @@
       <c r="K511" s="31"/>
     </row>
     <row r="516" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A516" s="41" t="s">
+      <c r="A516" s="44" t="s">
         <v>298</v>
       </c>
       <c r="B516" s="35"/>
       <c r="C516" s="35"/>
       <c r="D516" s="35"/>
-      <c r="E516" s="43"/>
+      <c r="E516" s="46"/>
       <c r="G516" s="33"/>
       <c r="H516" s="35" t="s">
         <v>299</v>
@@ -10232,11 +10424,11 @@
       <c r="K516" s="35"/>
     </row>
     <row r="517" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A517" s="42"/>
+      <c r="A517" s="45"/>
       <c r="B517" s="36"/>
       <c r="C517" s="36"/>
       <c r="D517" s="36"/>
-      <c r="E517" s="44"/>
+      <c r="E517" s="47"/>
       <c r="G517" s="34"/>
       <c r="H517" s="36"/>
       <c r="I517" s="36"/>
@@ -10333,10 +10525,10 @@
       <c r="K523" s="30"/>
     </row>
     <row r="524" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A524" s="45"/>
-      <c r="B524" s="46"/>
-      <c r="C524" s="46"/>
-      <c r="D524" s="47"/>
+      <c r="A524" s="41"/>
+      <c r="B524" s="42"/>
+      <c r="C524" s="42"/>
+      <c r="D524" s="43"/>
       <c r="H524" s="31"/>
       <c r="I524" s="31"/>
       <c r="J524" s="31"/>
@@ -10515,13 +10707,13 @@
       <c r="K535" s="31"/>
     </row>
     <row r="538" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A538" s="41" t="s">
+      <c r="A538" s="44" t="s">
         <v>300</v>
       </c>
       <c r="B538" s="35"/>
       <c r="C538" s="35"/>
       <c r="D538" s="35"/>
-      <c r="E538" s="43"/>
+      <c r="E538" s="46"/>
       <c r="G538" s="33"/>
       <c r="H538" s="35" t="s">
         <v>301</v>
@@ -10531,11 +10723,11 @@
       <c r="K538" s="35"/>
     </row>
     <row r="539" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A539" s="42"/>
+      <c r="A539" s="45"/>
       <c r="B539" s="36"/>
       <c r="C539" s="36"/>
       <c r="D539" s="36"/>
-      <c r="E539" s="44"/>
+      <c r="E539" s="47"/>
       <c r="G539" s="34"/>
       <c r="H539" s="36"/>
       <c r="I539" s="36"/>
@@ -10632,10 +10824,10 @@
       <c r="K545" s="30"/>
     </row>
     <row r="546" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A546" s="45"/>
-      <c r="B546" s="46"/>
-      <c r="C546" s="46"/>
-      <c r="D546" s="47"/>
+      <c r="A546" s="41"/>
+      <c r="B546" s="42"/>
+      <c r="C546" s="42"/>
+      <c r="D546" s="43"/>
       <c r="H546" s="31"/>
       <c r="I546" s="31"/>
       <c r="J546" s="31"/>
@@ -10815,402 +11007,576 @@
     </row>
   </sheetData>
   <mergeCells count="990">
-    <mergeCell ref="H545:K545"/>
-    <mergeCell ref="H546:K546"/>
-    <mergeCell ref="H547:K547"/>
-    <mergeCell ref="H548:K548"/>
-    <mergeCell ref="H555:K555"/>
-    <mergeCell ref="H556:I556"/>
-    <mergeCell ref="J556:K556"/>
-    <mergeCell ref="H557:I557"/>
-    <mergeCell ref="J557:K557"/>
-    <mergeCell ref="G538:G539"/>
-    <mergeCell ref="H538:K539"/>
-    <mergeCell ref="H541:I541"/>
-    <mergeCell ref="J541:K541"/>
-    <mergeCell ref="H542:I542"/>
-    <mergeCell ref="J542:K542"/>
-    <mergeCell ref="H543:I543"/>
-    <mergeCell ref="J543:K543"/>
-    <mergeCell ref="H544:I544"/>
-    <mergeCell ref="J544:K544"/>
-    <mergeCell ref="A545:D545"/>
-    <mergeCell ref="A546:D546"/>
-    <mergeCell ref="A547:D547"/>
-    <mergeCell ref="A548:D548"/>
-    <mergeCell ref="A555:D555"/>
-    <mergeCell ref="A556:B556"/>
-    <mergeCell ref="C556:D556"/>
-    <mergeCell ref="A557:B557"/>
-    <mergeCell ref="C557:D557"/>
-    <mergeCell ref="A538:D539"/>
-    <mergeCell ref="E538:E539"/>
-    <mergeCell ref="A541:B541"/>
-    <mergeCell ref="C541:D541"/>
-    <mergeCell ref="A542:B542"/>
-    <mergeCell ref="C542:D542"/>
-    <mergeCell ref="A543:B543"/>
-    <mergeCell ref="C543:D543"/>
-    <mergeCell ref="A544:B544"/>
-    <mergeCell ref="C544:D544"/>
-    <mergeCell ref="H523:K523"/>
-    <mergeCell ref="H524:K524"/>
-    <mergeCell ref="H525:K525"/>
-    <mergeCell ref="H526:K526"/>
-    <mergeCell ref="H533:K533"/>
-    <mergeCell ref="H534:I534"/>
-    <mergeCell ref="J534:K534"/>
-    <mergeCell ref="H535:I535"/>
-    <mergeCell ref="J535:K535"/>
-    <mergeCell ref="G516:G517"/>
-    <mergeCell ref="H516:K517"/>
-    <mergeCell ref="H519:I519"/>
-    <mergeCell ref="J519:K519"/>
-    <mergeCell ref="H520:I520"/>
-    <mergeCell ref="J520:K520"/>
-    <mergeCell ref="H521:I521"/>
-    <mergeCell ref="J521:K521"/>
-    <mergeCell ref="H522:I522"/>
-    <mergeCell ref="J522:K522"/>
-    <mergeCell ref="A523:D523"/>
-    <mergeCell ref="A524:D524"/>
-    <mergeCell ref="A525:D525"/>
-    <mergeCell ref="A526:D526"/>
-    <mergeCell ref="A533:D533"/>
-    <mergeCell ref="A534:B534"/>
-    <mergeCell ref="C534:D534"/>
-    <mergeCell ref="A535:B535"/>
-    <mergeCell ref="C535:D535"/>
-    <mergeCell ref="A516:D517"/>
-    <mergeCell ref="E516:E517"/>
-    <mergeCell ref="A519:B519"/>
-    <mergeCell ref="C519:D519"/>
-    <mergeCell ref="A520:B520"/>
-    <mergeCell ref="C520:D520"/>
-    <mergeCell ref="A521:B521"/>
-    <mergeCell ref="C521:D521"/>
-    <mergeCell ref="A522:B522"/>
-    <mergeCell ref="C522:D522"/>
-    <mergeCell ref="H499:K499"/>
-    <mergeCell ref="H500:K500"/>
-    <mergeCell ref="H501:K501"/>
-    <mergeCell ref="H502:K502"/>
-    <mergeCell ref="H509:K509"/>
-    <mergeCell ref="H510:I510"/>
-    <mergeCell ref="J510:K510"/>
-    <mergeCell ref="H511:I511"/>
-    <mergeCell ref="J511:K511"/>
-    <mergeCell ref="G492:G493"/>
-    <mergeCell ref="H492:K493"/>
-    <mergeCell ref="H495:I495"/>
-    <mergeCell ref="J495:K495"/>
-    <mergeCell ref="H496:I496"/>
-    <mergeCell ref="J496:K496"/>
-    <mergeCell ref="H497:I497"/>
-    <mergeCell ref="J497:K497"/>
-    <mergeCell ref="H498:I498"/>
-    <mergeCell ref="J498:K498"/>
-    <mergeCell ref="A499:D499"/>
-    <mergeCell ref="A500:D500"/>
-    <mergeCell ref="A501:D501"/>
-    <mergeCell ref="A502:D502"/>
-    <mergeCell ref="A509:D509"/>
-    <mergeCell ref="A510:B510"/>
-    <mergeCell ref="C510:D510"/>
-    <mergeCell ref="A511:B511"/>
-    <mergeCell ref="C511:D511"/>
-    <mergeCell ref="A492:D493"/>
-    <mergeCell ref="E492:E493"/>
-    <mergeCell ref="A495:B495"/>
-    <mergeCell ref="C495:D495"/>
-    <mergeCell ref="A496:B496"/>
-    <mergeCell ref="C496:D496"/>
-    <mergeCell ref="A497:B497"/>
-    <mergeCell ref="C497:D497"/>
-    <mergeCell ref="A498:B498"/>
-    <mergeCell ref="C498:D498"/>
-    <mergeCell ref="H476:K476"/>
-    <mergeCell ref="H477:K477"/>
-    <mergeCell ref="H478:K478"/>
-    <mergeCell ref="H479:K479"/>
-    <mergeCell ref="H486:K486"/>
-    <mergeCell ref="H487:I487"/>
-    <mergeCell ref="J487:K487"/>
-    <mergeCell ref="H488:I488"/>
-    <mergeCell ref="J488:K488"/>
-    <mergeCell ref="G469:G470"/>
-    <mergeCell ref="H469:K470"/>
-    <mergeCell ref="H472:I472"/>
-    <mergeCell ref="J472:K472"/>
-    <mergeCell ref="H473:I473"/>
-    <mergeCell ref="J473:K473"/>
-    <mergeCell ref="H474:I474"/>
-    <mergeCell ref="J474:K474"/>
-    <mergeCell ref="H475:I475"/>
-    <mergeCell ref="J475:K475"/>
-    <mergeCell ref="A476:D476"/>
-    <mergeCell ref="A477:D477"/>
-    <mergeCell ref="A478:D478"/>
-    <mergeCell ref="A479:D479"/>
-    <mergeCell ref="A486:D486"/>
-    <mergeCell ref="A487:B487"/>
-    <mergeCell ref="C487:D487"/>
-    <mergeCell ref="A488:B488"/>
-    <mergeCell ref="C488:D488"/>
-    <mergeCell ref="A469:D470"/>
-    <mergeCell ref="E469:E470"/>
-    <mergeCell ref="A472:B472"/>
-    <mergeCell ref="C472:D472"/>
-    <mergeCell ref="A473:B473"/>
-    <mergeCell ref="C473:D473"/>
-    <mergeCell ref="A474:B474"/>
-    <mergeCell ref="C474:D474"/>
-    <mergeCell ref="A475:B475"/>
-    <mergeCell ref="C475:D475"/>
-    <mergeCell ref="H454:K454"/>
-    <mergeCell ref="H456:K456"/>
-    <mergeCell ref="H464:K464"/>
-    <mergeCell ref="H465:I465"/>
-    <mergeCell ref="J465:K465"/>
-    <mergeCell ref="H466:I466"/>
-    <mergeCell ref="J466:K466"/>
-    <mergeCell ref="G447:G448"/>
-    <mergeCell ref="H447:K448"/>
-    <mergeCell ref="H450:I450"/>
-    <mergeCell ref="J450:K450"/>
-    <mergeCell ref="H451:I451"/>
-    <mergeCell ref="J451:K451"/>
-    <mergeCell ref="H452:I452"/>
-    <mergeCell ref="J452:K452"/>
-    <mergeCell ref="H453:I453"/>
-    <mergeCell ref="J453:K453"/>
-    <mergeCell ref="A454:D454"/>
-    <mergeCell ref="H455:K455"/>
-    <mergeCell ref="A456:D456"/>
-    <mergeCell ref="H457:K457"/>
-    <mergeCell ref="A464:D464"/>
-    <mergeCell ref="A465:B465"/>
-    <mergeCell ref="C465:D465"/>
-    <mergeCell ref="A466:B466"/>
-    <mergeCell ref="C466:D466"/>
-    <mergeCell ref="A447:D448"/>
-    <mergeCell ref="E447:E448"/>
-    <mergeCell ref="A450:B450"/>
-    <mergeCell ref="C450:D450"/>
-    <mergeCell ref="A451:B451"/>
-    <mergeCell ref="C451:D451"/>
-    <mergeCell ref="A452:B452"/>
-    <mergeCell ref="C452:D452"/>
-    <mergeCell ref="A453:B453"/>
-    <mergeCell ref="C453:D453"/>
-    <mergeCell ref="H432:K432"/>
-    <mergeCell ref="H433:K433"/>
-    <mergeCell ref="H434:K434"/>
-    <mergeCell ref="H435:K435"/>
-    <mergeCell ref="H442:K442"/>
-    <mergeCell ref="H443:I443"/>
-    <mergeCell ref="J443:K443"/>
-    <mergeCell ref="H444:I444"/>
-    <mergeCell ref="J444:K444"/>
-    <mergeCell ref="G425:G426"/>
-    <mergeCell ref="H425:K426"/>
-    <mergeCell ref="H428:I428"/>
-    <mergeCell ref="J428:K428"/>
-    <mergeCell ref="H429:I429"/>
-    <mergeCell ref="J429:K429"/>
-    <mergeCell ref="H430:I430"/>
-    <mergeCell ref="J430:K430"/>
-    <mergeCell ref="H431:I431"/>
-    <mergeCell ref="J431:K431"/>
-    <mergeCell ref="A432:D432"/>
-    <mergeCell ref="A433:D433"/>
-    <mergeCell ref="A434:D434"/>
-    <mergeCell ref="A435:D435"/>
-    <mergeCell ref="A442:D442"/>
-    <mergeCell ref="A443:B443"/>
-    <mergeCell ref="C443:D443"/>
-    <mergeCell ref="A444:B444"/>
-    <mergeCell ref="C444:D444"/>
-    <mergeCell ref="A425:D426"/>
-    <mergeCell ref="E425:E426"/>
-    <mergeCell ref="A428:B428"/>
-    <mergeCell ref="C428:D428"/>
-    <mergeCell ref="A429:B429"/>
-    <mergeCell ref="C429:D429"/>
-    <mergeCell ref="A430:B430"/>
-    <mergeCell ref="C430:D430"/>
-    <mergeCell ref="A431:B431"/>
-    <mergeCell ref="C431:D431"/>
-    <mergeCell ref="H410:K410"/>
-    <mergeCell ref="H411:K411"/>
-    <mergeCell ref="H412:K412"/>
-    <mergeCell ref="H413:K413"/>
-    <mergeCell ref="H420:K420"/>
-    <mergeCell ref="H421:I421"/>
-    <mergeCell ref="J421:K421"/>
-    <mergeCell ref="H422:I422"/>
-    <mergeCell ref="J422:K422"/>
-    <mergeCell ref="G403:G404"/>
-    <mergeCell ref="H403:K404"/>
-    <mergeCell ref="H406:I406"/>
-    <mergeCell ref="J406:K406"/>
-    <mergeCell ref="H407:I407"/>
-    <mergeCell ref="J407:K407"/>
-    <mergeCell ref="H408:I408"/>
-    <mergeCell ref="J408:K408"/>
-    <mergeCell ref="H409:I409"/>
-    <mergeCell ref="J409:K409"/>
-    <mergeCell ref="A410:D410"/>
-    <mergeCell ref="A411:D411"/>
-    <mergeCell ref="A412:D412"/>
-    <mergeCell ref="A413:D413"/>
-    <mergeCell ref="A420:D420"/>
-    <mergeCell ref="A421:B421"/>
-    <mergeCell ref="C421:D421"/>
-    <mergeCell ref="A422:B422"/>
-    <mergeCell ref="C422:D422"/>
-    <mergeCell ref="A403:D404"/>
-    <mergeCell ref="E403:E404"/>
-    <mergeCell ref="A406:B406"/>
-    <mergeCell ref="C406:D406"/>
-    <mergeCell ref="A407:B407"/>
-    <mergeCell ref="C407:D407"/>
-    <mergeCell ref="A408:B408"/>
-    <mergeCell ref="C408:D408"/>
-    <mergeCell ref="A409:B409"/>
-    <mergeCell ref="C409:D409"/>
-    <mergeCell ref="H345:K345"/>
-    <mergeCell ref="H346:K346"/>
-    <mergeCell ref="H347:K347"/>
-    <mergeCell ref="H348:K348"/>
-    <mergeCell ref="H355:K355"/>
-    <mergeCell ref="H356:I356"/>
-    <mergeCell ref="J356:K356"/>
-    <mergeCell ref="H357:I357"/>
-    <mergeCell ref="J357:K357"/>
-    <mergeCell ref="G338:G339"/>
-    <mergeCell ref="H338:K339"/>
-    <mergeCell ref="H341:I341"/>
-    <mergeCell ref="J341:K341"/>
-    <mergeCell ref="H342:I342"/>
-    <mergeCell ref="J342:K342"/>
-    <mergeCell ref="H343:I343"/>
-    <mergeCell ref="J343:K343"/>
-    <mergeCell ref="H344:I344"/>
-    <mergeCell ref="J344:K344"/>
-    <mergeCell ref="A345:D345"/>
-    <mergeCell ref="A346:D346"/>
-    <mergeCell ref="A347:D347"/>
-    <mergeCell ref="A348:D348"/>
-    <mergeCell ref="A355:D355"/>
-    <mergeCell ref="A356:B356"/>
-    <mergeCell ref="C356:D356"/>
-    <mergeCell ref="A357:B357"/>
-    <mergeCell ref="C357:D357"/>
-    <mergeCell ref="A338:D339"/>
-    <mergeCell ref="E338:E339"/>
-    <mergeCell ref="A341:B341"/>
-    <mergeCell ref="C341:D341"/>
-    <mergeCell ref="A342:B342"/>
-    <mergeCell ref="C342:D342"/>
-    <mergeCell ref="A343:B343"/>
-    <mergeCell ref="C343:D343"/>
-    <mergeCell ref="A344:B344"/>
-    <mergeCell ref="C344:D344"/>
-    <mergeCell ref="H302:K302"/>
-    <mergeCell ref="H303:K303"/>
-    <mergeCell ref="H304:K304"/>
-    <mergeCell ref="H305:K305"/>
-    <mergeCell ref="H312:K312"/>
-    <mergeCell ref="H313:I313"/>
-    <mergeCell ref="J313:K313"/>
-    <mergeCell ref="H314:I314"/>
-    <mergeCell ref="J314:K314"/>
-    <mergeCell ref="H319:I319"/>
-    <mergeCell ref="J319:K319"/>
-    <mergeCell ref="H320:I320"/>
-    <mergeCell ref="J320:K320"/>
-    <mergeCell ref="H321:I321"/>
-    <mergeCell ref="J321:K321"/>
-    <mergeCell ref="H322:I322"/>
-    <mergeCell ref="J322:K322"/>
-    <mergeCell ref="G316:G317"/>
-    <mergeCell ref="H316:K317"/>
-    <mergeCell ref="H295:K296"/>
-    <mergeCell ref="H298:I298"/>
-    <mergeCell ref="J298:K298"/>
-    <mergeCell ref="H299:I299"/>
-    <mergeCell ref="J299:K299"/>
-    <mergeCell ref="H300:I300"/>
-    <mergeCell ref="J300:K300"/>
-    <mergeCell ref="H301:I301"/>
-    <mergeCell ref="J301:K301"/>
-    <mergeCell ref="H323:K323"/>
-    <mergeCell ref="H324:K324"/>
-    <mergeCell ref="H325:K325"/>
-    <mergeCell ref="H326:K326"/>
-    <mergeCell ref="H333:K333"/>
-    <mergeCell ref="H334:I334"/>
-    <mergeCell ref="J334:K334"/>
-    <mergeCell ref="A324:D324"/>
-    <mergeCell ref="H335:I335"/>
-    <mergeCell ref="J335:K335"/>
-    <mergeCell ref="E316:E317"/>
-    <mergeCell ref="A319:B319"/>
-    <mergeCell ref="C319:D319"/>
-    <mergeCell ref="A320:B320"/>
-    <mergeCell ref="C320:D320"/>
-    <mergeCell ref="A335:B335"/>
-    <mergeCell ref="C335:D335"/>
-    <mergeCell ref="A321:B321"/>
-    <mergeCell ref="C321:D321"/>
-    <mergeCell ref="A322:B322"/>
-    <mergeCell ref="C322:D322"/>
-    <mergeCell ref="A323:D323"/>
-    <mergeCell ref="A334:B334"/>
-    <mergeCell ref="C334:D334"/>
-    <mergeCell ref="A303:D303"/>
-    <mergeCell ref="A325:D325"/>
-    <mergeCell ref="A326:D326"/>
-    <mergeCell ref="A333:D333"/>
-    <mergeCell ref="A302:D302"/>
-    <mergeCell ref="A304:D304"/>
-    <mergeCell ref="A305:D305"/>
-    <mergeCell ref="A312:D312"/>
-    <mergeCell ref="A313:B313"/>
-    <mergeCell ref="C313:D313"/>
-    <mergeCell ref="A314:B314"/>
-    <mergeCell ref="C314:D314"/>
-    <mergeCell ref="A316:D317"/>
-    <mergeCell ref="E274:E275"/>
-    <mergeCell ref="A277:B277"/>
-    <mergeCell ref="C277:D277"/>
-    <mergeCell ref="A278:B278"/>
-    <mergeCell ref="A300:B300"/>
-    <mergeCell ref="C300:D300"/>
-    <mergeCell ref="A301:B301"/>
-    <mergeCell ref="C301:D301"/>
-    <mergeCell ref="A295:D296"/>
-    <mergeCell ref="E295:E296"/>
-    <mergeCell ref="A298:B298"/>
-    <mergeCell ref="C298:D298"/>
-    <mergeCell ref="A299:B299"/>
-    <mergeCell ref="C299:D299"/>
-    <mergeCell ref="C278:D278"/>
-    <mergeCell ref="A279:B279"/>
-    <mergeCell ref="C279:D279"/>
-    <mergeCell ref="A280:B280"/>
-    <mergeCell ref="C280:D280"/>
-    <mergeCell ref="G295:G296"/>
-    <mergeCell ref="A281:D281"/>
-    <mergeCell ref="A282:D282"/>
-    <mergeCell ref="A283:D283"/>
-    <mergeCell ref="A284:D284"/>
-    <mergeCell ref="A291:D291"/>
-    <mergeCell ref="A292:B292"/>
-    <mergeCell ref="C292:D292"/>
-    <mergeCell ref="A293:B293"/>
-    <mergeCell ref="C293:D293"/>
+    <mergeCell ref="H388:K388"/>
+    <mergeCell ref="H389:K389"/>
+    <mergeCell ref="H390:K390"/>
+    <mergeCell ref="H391:K391"/>
+    <mergeCell ref="H398:K398"/>
+    <mergeCell ref="H399:I399"/>
+    <mergeCell ref="J399:K399"/>
+    <mergeCell ref="H400:I400"/>
+    <mergeCell ref="J400:K400"/>
+    <mergeCell ref="G381:G382"/>
+    <mergeCell ref="H381:K382"/>
+    <mergeCell ref="H384:I384"/>
+    <mergeCell ref="J384:K384"/>
+    <mergeCell ref="H385:I385"/>
+    <mergeCell ref="J385:K385"/>
+    <mergeCell ref="H386:I386"/>
+    <mergeCell ref="J386:K386"/>
+    <mergeCell ref="H387:I387"/>
+    <mergeCell ref="J387:K387"/>
+    <mergeCell ref="A388:D388"/>
+    <mergeCell ref="A389:D389"/>
+    <mergeCell ref="A390:D390"/>
+    <mergeCell ref="A391:D391"/>
+    <mergeCell ref="A398:D398"/>
+    <mergeCell ref="A399:B399"/>
+    <mergeCell ref="C399:D399"/>
+    <mergeCell ref="A400:B400"/>
+    <mergeCell ref="C400:D400"/>
+    <mergeCell ref="A381:D382"/>
+    <mergeCell ref="E381:E382"/>
+    <mergeCell ref="A384:B384"/>
+    <mergeCell ref="C384:D384"/>
+    <mergeCell ref="A385:B385"/>
+    <mergeCell ref="C385:D385"/>
+    <mergeCell ref="A386:B386"/>
+    <mergeCell ref="C386:D386"/>
+    <mergeCell ref="A387:B387"/>
+    <mergeCell ref="C387:D387"/>
+    <mergeCell ref="H367:K367"/>
+    <mergeCell ref="H368:K368"/>
+    <mergeCell ref="H369:K369"/>
+    <mergeCell ref="H370:K370"/>
+    <mergeCell ref="H377:K377"/>
+    <mergeCell ref="H378:I378"/>
+    <mergeCell ref="J378:K378"/>
+    <mergeCell ref="H379:I379"/>
+    <mergeCell ref="J379:K379"/>
+    <mergeCell ref="G360:G361"/>
+    <mergeCell ref="H360:K361"/>
+    <mergeCell ref="H363:I363"/>
+    <mergeCell ref="J363:K363"/>
+    <mergeCell ref="H364:I364"/>
+    <mergeCell ref="J364:K364"/>
+    <mergeCell ref="H365:I365"/>
+    <mergeCell ref="J365:K365"/>
+    <mergeCell ref="H366:I366"/>
+    <mergeCell ref="J366:K366"/>
+    <mergeCell ref="A367:D367"/>
+    <mergeCell ref="A368:D368"/>
+    <mergeCell ref="A369:D369"/>
+    <mergeCell ref="A370:D370"/>
+    <mergeCell ref="A377:D377"/>
+    <mergeCell ref="A378:B378"/>
+    <mergeCell ref="C378:D378"/>
+    <mergeCell ref="A379:B379"/>
+    <mergeCell ref="C379:D379"/>
+    <mergeCell ref="A360:D361"/>
+    <mergeCell ref="E360:E361"/>
+    <mergeCell ref="A363:B363"/>
+    <mergeCell ref="C363:D363"/>
+    <mergeCell ref="A364:B364"/>
+    <mergeCell ref="C364:D364"/>
+    <mergeCell ref="A365:B365"/>
+    <mergeCell ref="C365:D365"/>
+    <mergeCell ref="A366:B366"/>
+    <mergeCell ref="C366:D366"/>
+    <mergeCell ref="H238:K238"/>
+    <mergeCell ref="H239:K239"/>
+    <mergeCell ref="H240:K240"/>
+    <mergeCell ref="H241:K241"/>
+    <mergeCell ref="H248:K248"/>
+    <mergeCell ref="H249:I249"/>
+    <mergeCell ref="J249:K249"/>
+    <mergeCell ref="H250:I250"/>
+    <mergeCell ref="J250:K250"/>
+    <mergeCell ref="H231:K232"/>
+    <mergeCell ref="H234:I234"/>
+    <mergeCell ref="J234:K234"/>
+    <mergeCell ref="H235:I235"/>
+    <mergeCell ref="J235:K235"/>
+    <mergeCell ref="H236:I236"/>
+    <mergeCell ref="J236:K236"/>
+    <mergeCell ref="H237:I237"/>
+    <mergeCell ref="J237:K237"/>
+    <mergeCell ref="A238:D238"/>
+    <mergeCell ref="A239:D239"/>
+    <mergeCell ref="A240:D240"/>
+    <mergeCell ref="A241:D241"/>
+    <mergeCell ref="A248:D248"/>
+    <mergeCell ref="A249:B249"/>
+    <mergeCell ref="C249:D249"/>
+    <mergeCell ref="A250:B250"/>
+    <mergeCell ref="C250:D250"/>
+    <mergeCell ref="A231:D232"/>
+    <mergeCell ref="E231:E232"/>
+    <mergeCell ref="A234:B234"/>
+    <mergeCell ref="C234:D234"/>
+    <mergeCell ref="A235:B235"/>
+    <mergeCell ref="C235:D235"/>
+    <mergeCell ref="A236:B236"/>
+    <mergeCell ref="C236:D236"/>
+    <mergeCell ref="A237:B237"/>
+    <mergeCell ref="C237:D237"/>
+    <mergeCell ref="H217:K217"/>
+    <mergeCell ref="H218:K218"/>
+    <mergeCell ref="H219:K219"/>
+    <mergeCell ref="H220:K220"/>
+    <mergeCell ref="H227:K227"/>
+    <mergeCell ref="H228:I228"/>
+    <mergeCell ref="J228:K228"/>
+    <mergeCell ref="H229:I229"/>
+    <mergeCell ref="J229:K229"/>
+    <mergeCell ref="H210:K211"/>
+    <mergeCell ref="L210:L211"/>
+    <mergeCell ref="H213:I213"/>
+    <mergeCell ref="J213:K213"/>
+    <mergeCell ref="H214:I214"/>
+    <mergeCell ref="J214:K214"/>
+    <mergeCell ref="H215:I215"/>
+    <mergeCell ref="J215:K215"/>
+    <mergeCell ref="H216:I216"/>
+    <mergeCell ref="J216:K216"/>
+    <mergeCell ref="A217:D217"/>
+    <mergeCell ref="A218:D218"/>
+    <mergeCell ref="A219:D219"/>
+    <mergeCell ref="A220:D220"/>
+    <mergeCell ref="A227:D227"/>
+    <mergeCell ref="A228:B228"/>
+    <mergeCell ref="C228:D228"/>
+    <mergeCell ref="A229:B229"/>
+    <mergeCell ref="C229:D229"/>
+    <mergeCell ref="A210:D211"/>
+    <mergeCell ref="E210:E211"/>
+    <mergeCell ref="A213:B213"/>
+    <mergeCell ref="C213:D213"/>
+    <mergeCell ref="A214:B214"/>
+    <mergeCell ref="C214:D214"/>
+    <mergeCell ref="A215:B215"/>
+    <mergeCell ref="C215:D215"/>
+    <mergeCell ref="A216:B216"/>
+    <mergeCell ref="C216:D216"/>
+    <mergeCell ref="A207:B207"/>
+    <mergeCell ref="C207:D207"/>
+    <mergeCell ref="A208:B208"/>
+    <mergeCell ref="C208:D208"/>
+    <mergeCell ref="H189:K190"/>
+    <mergeCell ref="L189:L190"/>
+    <mergeCell ref="H192:I192"/>
+    <mergeCell ref="J192:K192"/>
+    <mergeCell ref="H193:I193"/>
+    <mergeCell ref="J193:K193"/>
+    <mergeCell ref="H194:I194"/>
+    <mergeCell ref="J194:K194"/>
+    <mergeCell ref="H195:I195"/>
+    <mergeCell ref="J195:K195"/>
+    <mergeCell ref="H196:K196"/>
+    <mergeCell ref="H197:K197"/>
+    <mergeCell ref="H198:K198"/>
+    <mergeCell ref="H199:K199"/>
+    <mergeCell ref="H206:K206"/>
+    <mergeCell ref="H207:I207"/>
+    <mergeCell ref="J207:K207"/>
+    <mergeCell ref="H208:I208"/>
+    <mergeCell ref="J208:K208"/>
+    <mergeCell ref="A194:B194"/>
+    <mergeCell ref="C194:D194"/>
+    <mergeCell ref="A195:B195"/>
+    <mergeCell ref="C195:D195"/>
+    <mergeCell ref="A196:D196"/>
+    <mergeCell ref="A197:D197"/>
+    <mergeCell ref="A198:D198"/>
+    <mergeCell ref="A199:D199"/>
+    <mergeCell ref="A206:D206"/>
+    <mergeCell ref="G168:G169"/>
+    <mergeCell ref="A187:B187"/>
+    <mergeCell ref="C187:D187"/>
+    <mergeCell ref="A168:D169"/>
+    <mergeCell ref="E168:E169"/>
+    <mergeCell ref="A171:B171"/>
+    <mergeCell ref="C171:D171"/>
+    <mergeCell ref="A172:B172"/>
+    <mergeCell ref="C172:D172"/>
+    <mergeCell ref="A173:B173"/>
+    <mergeCell ref="C173:D173"/>
+    <mergeCell ref="A174:B174"/>
+    <mergeCell ref="C174:D174"/>
+    <mergeCell ref="G189:G190"/>
+    <mergeCell ref="G147:G148"/>
+    <mergeCell ref="A189:D190"/>
+    <mergeCell ref="E189:E190"/>
+    <mergeCell ref="A192:B192"/>
+    <mergeCell ref="C192:D192"/>
+    <mergeCell ref="A193:B193"/>
+    <mergeCell ref="C193:D193"/>
+    <mergeCell ref="H175:K175"/>
+    <mergeCell ref="H176:K176"/>
+    <mergeCell ref="H177:K177"/>
+    <mergeCell ref="H178:K178"/>
+    <mergeCell ref="H185:K185"/>
+    <mergeCell ref="H186:I186"/>
+    <mergeCell ref="J186:K186"/>
+    <mergeCell ref="H187:I187"/>
+    <mergeCell ref="J187:K187"/>
+    <mergeCell ref="H168:K169"/>
+    <mergeCell ref="A175:D175"/>
+    <mergeCell ref="A176:D176"/>
+    <mergeCell ref="A177:D177"/>
+    <mergeCell ref="A178:D178"/>
+    <mergeCell ref="A185:D185"/>
+    <mergeCell ref="A186:B186"/>
+    <mergeCell ref="C186:D186"/>
+    <mergeCell ref="L168:L169"/>
+    <mergeCell ref="H171:I171"/>
+    <mergeCell ref="J171:K171"/>
+    <mergeCell ref="H172:I172"/>
+    <mergeCell ref="J172:K172"/>
+    <mergeCell ref="H173:I173"/>
+    <mergeCell ref="J173:K173"/>
+    <mergeCell ref="H174:I174"/>
+    <mergeCell ref="J174:K174"/>
+    <mergeCell ref="H154:K154"/>
+    <mergeCell ref="H155:K155"/>
+    <mergeCell ref="H156:K156"/>
+    <mergeCell ref="H157:K157"/>
+    <mergeCell ref="H164:K164"/>
+    <mergeCell ref="H165:I165"/>
+    <mergeCell ref="J165:K165"/>
+    <mergeCell ref="H166:I166"/>
+    <mergeCell ref="J166:K166"/>
+    <mergeCell ref="H147:K148"/>
+    <mergeCell ref="L147:L148"/>
+    <mergeCell ref="H150:I150"/>
+    <mergeCell ref="J150:K150"/>
+    <mergeCell ref="H151:I151"/>
+    <mergeCell ref="J151:K151"/>
+    <mergeCell ref="H152:I152"/>
+    <mergeCell ref="J152:K152"/>
+    <mergeCell ref="H153:I153"/>
+    <mergeCell ref="J153:K153"/>
+    <mergeCell ref="A154:D154"/>
+    <mergeCell ref="A155:D155"/>
+    <mergeCell ref="A156:D156"/>
+    <mergeCell ref="A157:D157"/>
+    <mergeCell ref="A164:D164"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="C165:D165"/>
+    <mergeCell ref="A166:B166"/>
+    <mergeCell ref="C166:D166"/>
+    <mergeCell ref="A147:D148"/>
+    <mergeCell ref="E147:E148"/>
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="C150:D150"/>
+    <mergeCell ref="A151:B151"/>
+    <mergeCell ref="C151:D151"/>
+    <mergeCell ref="A152:B152"/>
+    <mergeCell ref="C152:D152"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="C153:D153"/>
+    <mergeCell ref="L126:L127"/>
+    <mergeCell ref="H129:I129"/>
+    <mergeCell ref="J129:K129"/>
+    <mergeCell ref="H130:I130"/>
+    <mergeCell ref="J130:K130"/>
+    <mergeCell ref="H131:I131"/>
+    <mergeCell ref="J131:K131"/>
+    <mergeCell ref="H132:I132"/>
+    <mergeCell ref="J132:K132"/>
+    <mergeCell ref="H126:K127"/>
+    <mergeCell ref="H133:K133"/>
+    <mergeCell ref="H134:K134"/>
+    <mergeCell ref="H135:K135"/>
+    <mergeCell ref="H136:K136"/>
+    <mergeCell ref="H143:K143"/>
+    <mergeCell ref="H144:I144"/>
+    <mergeCell ref="J144:K144"/>
+    <mergeCell ref="H145:I145"/>
+    <mergeCell ref="J145:K145"/>
+    <mergeCell ref="A133:D133"/>
+    <mergeCell ref="A134:D134"/>
+    <mergeCell ref="A135:D135"/>
+    <mergeCell ref="A136:D136"/>
+    <mergeCell ref="A143:D143"/>
+    <mergeCell ref="A144:B144"/>
+    <mergeCell ref="C144:D144"/>
+    <mergeCell ref="A145:B145"/>
+    <mergeCell ref="C145:D145"/>
+    <mergeCell ref="A126:D127"/>
+    <mergeCell ref="E126:E127"/>
+    <mergeCell ref="A129:B129"/>
+    <mergeCell ref="C129:D129"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="C130:D130"/>
+    <mergeCell ref="A131:B131"/>
+    <mergeCell ref="C131:D131"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="C132:D132"/>
+    <mergeCell ref="H112:K112"/>
+    <mergeCell ref="H113:K113"/>
+    <mergeCell ref="H114:K114"/>
+    <mergeCell ref="H115:K115"/>
+    <mergeCell ref="H122:K122"/>
+    <mergeCell ref="H123:I123"/>
+    <mergeCell ref="J123:K123"/>
+    <mergeCell ref="H124:I124"/>
+    <mergeCell ref="J124:K124"/>
+    <mergeCell ref="G105:G106"/>
+    <mergeCell ref="H105:K106"/>
+    <mergeCell ref="H108:I108"/>
+    <mergeCell ref="J108:K108"/>
+    <mergeCell ref="H109:I109"/>
+    <mergeCell ref="J109:K109"/>
+    <mergeCell ref="H110:I110"/>
+    <mergeCell ref="J110:K110"/>
+    <mergeCell ref="H111:I111"/>
+    <mergeCell ref="J111:K111"/>
+    <mergeCell ref="A112:D112"/>
+    <mergeCell ref="A113:D113"/>
+    <mergeCell ref="A114:D114"/>
+    <mergeCell ref="A115:D115"/>
+    <mergeCell ref="A122:D122"/>
+    <mergeCell ref="A123:B123"/>
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="A124:B124"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="A105:D106"/>
+    <mergeCell ref="E105:E106"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="A109:B109"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="A110:B110"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="A111:B111"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="H104:I104"/>
+    <mergeCell ref="J104:K104"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="A95:D95"/>
+    <mergeCell ref="H95:K95"/>
+    <mergeCell ref="A102:D102"/>
+    <mergeCell ref="H102:K102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="H103:I103"/>
+    <mergeCell ref="J103:K103"/>
+    <mergeCell ref="F1:F1048576"/>
+    <mergeCell ref="A92:D92"/>
+    <mergeCell ref="H92:K92"/>
+    <mergeCell ref="A93:D93"/>
+    <mergeCell ref="H93:K93"/>
+    <mergeCell ref="A94:D94"/>
+    <mergeCell ref="H94:K94"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="H90:I90"/>
+    <mergeCell ref="J90:K90"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="H91:I91"/>
+    <mergeCell ref="J91:K91"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="H88:I88"/>
+    <mergeCell ref="J88:K88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="J89:K89"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="H83:I83"/>
+    <mergeCell ref="J83:K83"/>
+    <mergeCell ref="A85:D86"/>
+    <mergeCell ref="H85:K86"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="G85:G86"/>
+    <mergeCell ref="A74:D74"/>
+    <mergeCell ref="H74:K74"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="H81:K81"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="H82:I82"/>
+    <mergeCell ref="J82:K82"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="H71:K71"/>
+    <mergeCell ref="A72:D72"/>
+    <mergeCell ref="H72:K72"/>
+    <mergeCell ref="A73:D73"/>
+    <mergeCell ref="H73:K73"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="H69:I69"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="J67:K67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="H68:I68"/>
+    <mergeCell ref="J68:K68"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="J62:K62"/>
+    <mergeCell ref="A64:D65"/>
+    <mergeCell ref="H64:K65"/>
+    <mergeCell ref="E64:E65"/>
+    <mergeCell ref="G64:G65"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="H60:K60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="J61:K61"/>
+    <mergeCell ref="A51:D51"/>
+    <mergeCell ref="H51:K51"/>
+    <mergeCell ref="A52:D52"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="H53:K53"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="H49:I49"/>
+    <mergeCell ref="J49:K49"/>
+    <mergeCell ref="A50:D50"/>
+    <mergeCell ref="H50:K50"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="H1:K2"/>
+    <mergeCell ref="A22:D23"/>
+    <mergeCell ref="H22:K23"/>
+    <mergeCell ref="H39:K39"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="H29:K29"/>
+    <mergeCell ref="H30:K30"/>
+    <mergeCell ref="H31:K31"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="A253:D254"/>
+    <mergeCell ref="E253:E254"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="A43:D44"/>
+    <mergeCell ref="H43:K44"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="H253:K254"/>
+    <mergeCell ref="H256:I256"/>
+    <mergeCell ref="J256:K256"/>
+    <mergeCell ref="H257:I257"/>
+    <mergeCell ref="J257:K257"/>
+    <mergeCell ref="H258:I258"/>
+    <mergeCell ref="J258:K258"/>
+    <mergeCell ref="H259:I259"/>
+    <mergeCell ref="J259:K259"/>
+    <mergeCell ref="H274:K275"/>
+    <mergeCell ref="A256:B256"/>
+    <mergeCell ref="C256:D256"/>
+    <mergeCell ref="A257:B257"/>
+    <mergeCell ref="C257:D257"/>
+    <mergeCell ref="A258:B258"/>
+    <mergeCell ref="C258:D258"/>
+    <mergeCell ref="A259:B259"/>
+    <mergeCell ref="C259:D259"/>
+    <mergeCell ref="H270:K270"/>
+    <mergeCell ref="H271:I271"/>
+    <mergeCell ref="J271:K271"/>
+    <mergeCell ref="H272:I272"/>
+    <mergeCell ref="J272:K272"/>
+    <mergeCell ref="A260:D260"/>
+    <mergeCell ref="A261:D261"/>
+    <mergeCell ref="A262:D262"/>
+    <mergeCell ref="A263:D263"/>
+    <mergeCell ref="A270:D270"/>
+    <mergeCell ref="A271:B271"/>
+    <mergeCell ref="C271:D271"/>
+    <mergeCell ref="A272:B272"/>
+    <mergeCell ref="C272:D272"/>
+    <mergeCell ref="A274:D275"/>
     <mergeCell ref="H282:K282"/>
     <mergeCell ref="H283:K283"/>
     <mergeCell ref="H284:K284"/>
@@ -11235,576 +11601,402 @@
     <mergeCell ref="H261:K261"/>
     <mergeCell ref="H262:K262"/>
     <mergeCell ref="H263:K263"/>
-    <mergeCell ref="H274:K275"/>
-    <mergeCell ref="A256:B256"/>
-    <mergeCell ref="C256:D256"/>
-    <mergeCell ref="A257:B257"/>
-    <mergeCell ref="C257:D257"/>
-    <mergeCell ref="A258:B258"/>
-    <mergeCell ref="C258:D258"/>
-    <mergeCell ref="A259:B259"/>
-    <mergeCell ref="C259:D259"/>
-    <mergeCell ref="H270:K270"/>
-    <mergeCell ref="H271:I271"/>
-    <mergeCell ref="J271:K271"/>
-    <mergeCell ref="H272:I272"/>
-    <mergeCell ref="J272:K272"/>
-    <mergeCell ref="A260:D260"/>
-    <mergeCell ref="A261:D261"/>
-    <mergeCell ref="A262:D262"/>
-    <mergeCell ref="A263:D263"/>
-    <mergeCell ref="A270:D270"/>
-    <mergeCell ref="A271:B271"/>
-    <mergeCell ref="C271:D271"/>
-    <mergeCell ref="A272:B272"/>
-    <mergeCell ref="C272:D272"/>
-    <mergeCell ref="A274:D275"/>
-    <mergeCell ref="H253:K254"/>
-    <mergeCell ref="H256:I256"/>
-    <mergeCell ref="J256:K256"/>
-    <mergeCell ref="H257:I257"/>
-    <mergeCell ref="J257:K257"/>
-    <mergeCell ref="H258:I258"/>
-    <mergeCell ref="J258:K258"/>
-    <mergeCell ref="H259:I259"/>
-    <mergeCell ref="J259:K259"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="A253:D254"/>
-    <mergeCell ref="E253:E254"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="A43:D44"/>
-    <mergeCell ref="H43:K44"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="H1:K2"/>
-    <mergeCell ref="A22:D23"/>
-    <mergeCell ref="H22:K23"/>
-    <mergeCell ref="H39:K39"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="H29:K29"/>
-    <mergeCell ref="H30:K30"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="A50:D50"/>
-    <mergeCell ref="H50:K50"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="H60:K60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="J61:K61"/>
-    <mergeCell ref="A51:D51"/>
-    <mergeCell ref="H51:K51"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="H53:K53"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="H67:I67"/>
-    <mergeCell ref="J67:K67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="H68:I68"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="J62:K62"/>
-    <mergeCell ref="A64:D65"/>
-    <mergeCell ref="H64:K65"/>
-    <mergeCell ref="E64:E65"/>
-    <mergeCell ref="G64:G65"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="H71:K71"/>
-    <mergeCell ref="A72:D72"/>
-    <mergeCell ref="H72:K72"/>
-    <mergeCell ref="A73:D73"/>
-    <mergeCell ref="H73:K73"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="H69:I69"/>
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="H70:I70"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="H83:I83"/>
-    <mergeCell ref="J83:K83"/>
-    <mergeCell ref="A85:D86"/>
-    <mergeCell ref="H85:K86"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="G85:G86"/>
-    <mergeCell ref="A74:D74"/>
-    <mergeCell ref="H74:K74"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="H81:K81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="H82:I82"/>
-    <mergeCell ref="J82:K82"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="H90:I90"/>
-    <mergeCell ref="J90:K90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="H91:I91"/>
-    <mergeCell ref="J91:K91"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="H88:I88"/>
-    <mergeCell ref="J88:K88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="J89:K89"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="H104:I104"/>
-    <mergeCell ref="J104:K104"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="A95:D95"/>
-    <mergeCell ref="H95:K95"/>
-    <mergeCell ref="A102:D102"/>
-    <mergeCell ref="H102:K102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="H103:I103"/>
-    <mergeCell ref="J103:K103"/>
-    <mergeCell ref="F1:F1048576"/>
-    <mergeCell ref="A92:D92"/>
-    <mergeCell ref="H92:K92"/>
-    <mergeCell ref="A93:D93"/>
-    <mergeCell ref="H93:K93"/>
-    <mergeCell ref="A94:D94"/>
-    <mergeCell ref="H94:K94"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A105:D106"/>
-    <mergeCell ref="E105:E106"/>
-    <mergeCell ref="A108:B108"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="A109:B109"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="A110:B110"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="A111:B111"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="A112:D112"/>
-    <mergeCell ref="A113:D113"/>
-    <mergeCell ref="A114:D114"/>
-    <mergeCell ref="A115:D115"/>
-    <mergeCell ref="A122:D122"/>
-    <mergeCell ref="A123:B123"/>
-    <mergeCell ref="C123:D123"/>
-    <mergeCell ref="A124:B124"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="G105:G106"/>
-    <mergeCell ref="H105:K106"/>
-    <mergeCell ref="H108:I108"/>
-    <mergeCell ref="J108:K108"/>
-    <mergeCell ref="H109:I109"/>
-    <mergeCell ref="J109:K109"/>
-    <mergeCell ref="H110:I110"/>
-    <mergeCell ref="J110:K110"/>
-    <mergeCell ref="H111:I111"/>
-    <mergeCell ref="J111:K111"/>
-    <mergeCell ref="H112:K112"/>
-    <mergeCell ref="H113:K113"/>
-    <mergeCell ref="H114:K114"/>
-    <mergeCell ref="H115:K115"/>
-    <mergeCell ref="H122:K122"/>
-    <mergeCell ref="H123:I123"/>
-    <mergeCell ref="J123:K123"/>
-    <mergeCell ref="H124:I124"/>
-    <mergeCell ref="J124:K124"/>
-    <mergeCell ref="A126:D127"/>
-    <mergeCell ref="E126:E127"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="C129:D129"/>
-    <mergeCell ref="A130:B130"/>
-    <mergeCell ref="C130:D130"/>
-    <mergeCell ref="A131:B131"/>
-    <mergeCell ref="C131:D131"/>
-    <mergeCell ref="A132:B132"/>
-    <mergeCell ref="C132:D132"/>
-    <mergeCell ref="A133:D133"/>
-    <mergeCell ref="A134:D134"/>
-    <mergeCell ref="A135:D135"/>
-    <mergeCell ref="A136:D136"/>
-    <mergeCell ref="A143:D143"/>
-    <mergeCell ref="A144:B144"/>
-    <mergeCell ref="C144:D144"/>
-    <mergeCell ref="A145:B145"/>
-    <mergeCell ref="C145:D145"/>
-    <mergeCell ref="H133:K133"/>
-    <mergeCell ref="H134:K134"/>
-    <mergeCell ref="H135:K135"/>
-    <mergeCell ref="H136:K136"/>
-    <mergeCell ref="H143:K143"/>
-    <mergeCell ref="H144:I144"/>
-    <mergeCell ref="J144:K144"/>
-    <mergeCell ref="H145:I145"/>
-    <mergeCell ref="J145:K145"/>
-    <mergeCell ref="L126:L127"/>
-    <mergeCell ref="H129:I129"/>
-    <mergeCell ref="J129:K129"/>
-    <mergeCell ref="H130:I130"/>
-    <mergeCell ref="J130:K130"/>
-    <mergeCell ref="H131:I131"/>
-    <mergeCell ref="J131:K131"/>
-    <mergeCell ref="H132:I132"/>
-    <mergeCell ref="J132:K132"/>
-    <mergeCell ref="H126:K127"/>
-    <mergeCell ref="A147:D148"/>
-    <mergeCell ref="E147:E148"/>
-    <mergeCell ref="A150:B150"/>
-    <mergeCell ref="C150:D150"/>
-    <mergeCell ref="A151:B151"/>
-    <mergeCell ref="C151:D151"/>
-    <mergeCell ref="A152:B152"/>
-    <mergeCell ref="C152:D152"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="C153:D153"/>
-    <mergeCell ref="A154:D154"/>
-    <mergeCell ref="A155:D155"/>
-    <mergeCell ref="A156:D156"/>
-    <mergeCell ref="A157:D157"/>
-    <mergeCell ref="A164:D164"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="C165:D165"/>
-    <mergeCell ref="A166:B166"/>
-    <mergeCell ref="C166:D166"/>
-    <mergeCell ref="H147:K148"/>
-    <mergeCell ref="L147:L148"/>
-    <mergeCell ref="H150:I150"/>
-    <mergeCell ref="J150:K150"/>
-    <mergeCell ref="H151:I151"/>
-    <mergeCell ref="J151:K151"/>
-    <mergeCell ref="H152:I152"/>
-    <mergeCell ref="J152:K152"/>
-    <mergeCell ref="H153:I153"/>
-    <mergeCell ref="J153:K153"/>
-    <mergeCell ref="H154:K154"/>
-    <mergeCell ref="H155:K155"/>
-    <mergeCell ref="H156:K156"/>
-    <mergeCell ref="H157:K157"/>
-    <mergeCell ref="H164:K164"/>
-    <mergeCell ref="H165:I165"/>
-    <mergeCell ref="J165:K165"/>
-    <mergeCell ref="H166:I166"/>
-    <mergeCell ref="J166:K166"/>
-    <mergeCell ref="L168:L169"/>
-    <mergeCell ref="H171:I171"/>
-    <mergeCell ref="J171:K171"/>
-    <mergeCell ref="H172:I172"/>
-    <mergeCell ref="J172:K172"/>
-    <mergeCell ref="H173:I173"/>
-    <mergeCell ref="J173:K173"/>
-    <mergeCell ref="H174:I174"/>
-    <mergeCell ref="J174:K174"/>
-    <mergeCell ref="G147:G148"/>
-    <mergeCell ref="A189:D190"/>
-    <mergeCell ref="E189:E190"/>
-    <mergeCell ref="A192:B192"/>
-    <mergeCell ref="C192:D192"/>
-    <mergeCell ref="A193:B193"/>
-    <mergeCell ref="C193:D193"/>
-    <mergeCell ref="H175:K175"/>
-    <mergeCell ref="H176:K176"/>
-    <mergeCell ref="H177:K177"/>
-    <mergeCell ref="H178:K178"/>
-    <mergeCell ref="H185:K185"/>
-    <mergeCell ref="H186:I186"/>
-    <mergeCell ref="J186:K186"/>
-    <mergeCell ref="H187:I187"/>
-    <mergeCell ref="J187:K187"/>
-    <mergeCell ref="H168:K169"/>
-    <mergeCell ref="A175:D175"/>
-    <mergeCell ref="A176:D176"/>
-    <mergeCell ref="A177:D177"/>
-    <mergeCell ref="A178:D178"/>
-    <mergeCell ref="A185:D185"/>
-    <mergeCell ref="A186:B186"/>
-    <mergeCell ref="C186:D186"/>
-    <mergeCell ref="C194:D194"/>
-    <mergeCell ref="A195:B195"/>
-    <mergeCell ref="C195:D195"/>
-    <mergeCell ref="A196:D196"/>
-    <mergeCell ref="A197:D197"/>
-    <mergeCell ref="A198:D198"/>
-    <mergeCell ref="A199:D199"/>
-    <mergeCell ref="A206:D206"/>
-    <mergeCell ref="G168:G169"/>
-    <mergeCell ref="A187:B187"/>
-    <mergeCell ref="C187:D187"/>
-    <mergeCell ref="A168:D169"/>
-    <mergeCell ref="E168:E169"/>
-    <mergeCell ref="A171:B171"/>
-    <mergeCell ref="C171:D171"/>
-    <mergeCell ref="A172:B172"/>
-    <mergeCell ref="C172:D172"/>
-    <mergeCell ref="A173:B173"/>
-    <mergeCell ref="C173:D173"/>
-    <mergeCell ref="A174:B174"/>
-    <mergeCell ref="C174:D174"/>
-    <mergeCell ref="G189:G190"/>
-    <mergeCell ref="A207:B207"/>
-    <mergeCell ref="C207:D207"/>
-    <mergeCell ref="A208:B208"/>
-    <mergeCell ref="C208:D208"/>
-    <mergeCell ref="H189:K190"/>
-    <mergeCell ref="L189:L190"/>
-    <mergeCell ref="H192:I192"/>
-    <mergeCell ref="J192:K192"/>
-    <mergeCell ref="H193:I193"/>
-    <mergeCell ref="J193:K193"/>
-    <mergeCell ref="H194:I194"/>
-    <mergeCell ref="J194:K194"/>
-    <mergeCell ref="H195:I195"/>
-    <mergeCell ref="J195:K195"/>
-    <mergeCell ref="H196:K196"/>
-    <mergeCell ref="H197:K197"/>
-    <mergeCell ref="H198:K198"/>
-    <mergeCell ref="H199:K199"/>
-    <mergeCell ref="H206:K206"/>
-    <mergeCell ref="H207:I207"/>
-    <mergeCell ref="J207:K207"/>
-    <mergeCell ref="H208:I208"/>
-    <mergeCell ref="J208:K208"/>
-    <mergeCell ref="A194:B194"/>
-    <mergeCell ref="A210:D211"/>
-    <mergeCell ref="E210:E211"/>
-    <mergeCell ref="A213:B213"/>
-    <mergeCell ref="C213:D213"/>
-    <mergeCell ref="A214:B214"/>
-    <mergeCell ref="C214:D214"/>
-    <mergeCell ref="A215:B215"/>
-    <mergeCell ref="C215:D215"/>
-    <mergeCell ref="A216:B216"/>
-    <mergeCell ref="C216:D216"/>
-    <mergeCell ref="A217:D217"/>
-    <mergeCell ref="A218:D218"/>
-    <mergeCell ref="A219:D219"/>
-    <mergeCell ref="A220:D220"/>
-    <mergeCell ref="A227:D227"/>
-    <mergeCell ref="A228:B228"/>
-    <mergeCell ref="C228:D228"/>
-    <mergeCell ref="A229:B229"/>
-    <mergeCell ref="C229:D229"/>
-    <mergeCell ref="H210:K211"/>
-    <mergeCell ref="L210:L211"/>
-    <mergeCell ref="H213:I213"/>
-    <mergeCell ref="J213:K213"/>
-    <mergeCell ref="H214:I214"/>
-    <mergeCell ref="J214:K214"/>
-    <mergeCell ref="H215:I215"/>
-    <mergeCell ref="J215:K215"/>
-    <mergeCell ref="H216:I216"/>
-    <mergeCell ref="J216:K216"/>
-    <mergeCell ref="H217:K217"/>
-    <mergeCell ref="H218:K218"/>
-    <mergeCell ref="H219:K219"/>
-    <mergeCell ref="H220:K220"/>
-    <mergeCell ref="H227:K227"/>
-    <mergeCell ref="H228:I228"/>
-    <mergeCell ref="J228:K228"/>
-    <mergeCell ref="H229:I229"/>
-    <mergeCell ref="J229:K229"/>
-    <mergeCell ref="A231:D232"/>
-    <mergeCell ref="E231:E232"/>
-    <mergeCell ref="A234:B234"/>
-    <mergeCell ref="C234:D234"/>
-    <mergeCell ref="A235:B235"/>
-    <mergeCell ref="C235:D235"/>
-    <mergeCell ref="A236:B236"/>
-    <mergeCell ref="C236:D236"/>
-    <mergeCell ref="A237:B237"/>
-    <mergeCell ref="C237:D237"/>
-    <mergeCell ref="A238:D238"/>
-    <mergeCell ref="A239:D239"/>
-    <mergeCell ref="A240:D240"/>
-    <mergeCell ref="A241:D241"/>
-    <mergeCell ref="A248:D248"/>
-    <mergeCell ref="A249:B249"/>
-    <mergeCell ref="C249:D249"/>
-    <mergeCell ref="A250:B250"/>
-    <mergeCell ref="C250:D250"/>
-    <mergeCell ref="H231:K232"/>
-    <mergeCell ref="H234:I234"/>
-    <mergeCell ref="J234:K234"/>
-    <mergeCell ref="H235:I235"/>
-    <mergeCell ref="J235:K235"/>
-    <mergeCell ref="H236:I236"/>
-    <mergeCell ref="J236:K236"/>
-    <mergeCell ref="H237:I237"/>
-    <mergeCell ref="J237:K237"/>
-    <mergeCell ref="H238:K238"/>
-    <mergeCell ref="H239:K239"/>
-    <mergeCell ref="H240:K240"/>
-    <mergeCell ref="H241:K241"/>
-    <mergeCell ref="H248:K248"/>
-    <mergeCell ref="H249:I249"/>
-    <mergeCell ref="J249:K249"/>
-    <mergeCell ref="H250:I250"/>
-    <mergeCell ref="J250:K250"/>
-    <mergeCell ref="A360:D361"/>
-    <mergeCell ref="E360:E361"/>
-    <mergeCell ref="A363:B363"/>
-    <mergeCell ref="C363:D363"/>
-    <mergeCell ref="A364:B364"/>
-    <mergeCell ref="C364:D364"/>
-    <mergeCell ref="A365:B365"/>
-    <mergeCell ref="C365:D365"/>
-    <mergeCell ref="A366:B366"/>
-    <mergeCell ref="C366:D366"/>
-    <mergeCell ref="A367:D367"/>
-    <mergeCell ref="A368:D368"/>
-    <mergeCell ref="A369:D369"/>
-    <mergeCell ref="A370:D370"/>
-    <mergeCell ref="A377:D377"/>
-    <mergeCell ref="A378:B378"/>
-    <mergeCell ref="C378:D378"/>
-    <mergeCell ref="A379:B379"/>
-    <mergeCell ref="C379:D379"/>
-    <mergeCell ref="G360:G361"/>
-    <mergeCell ref="H360:K361"/>
-    <mergeCell ref="H363:I363"/>
-    <mergeCell ref="J363:K363"/>
-    <mergeCell ref="H364:I364"/>
-    <mergeCell ref="J364:K364"/>
-    <mergeCell ref="H365:I365"/>
-    <mergeCell ref="J365:K365"/>
-    <mergeCell ref="H366:I366"/>
-    <mergeCell ref="J366:K366"/>
-    <mergeCell ref="H367:K367"/>
-    <mergeCell ref="H368:K368"/>
-    <mergeCell ref="H369:K369"/>
-    <mergeCell ref="H370:K370"/>
-    <mergeCell ref="H377:K377"/>
-    <mergeCell ref="H378:I378"/>
-    <mergeCell ref="J378:K378"/>
-    <mergeCell ref="H379:I379"/>
-    <mergeCell ref="J379:K379"/>
-    <mergeCell ref="A381:D382"/>
-    <mergeCell ref="E381:E382"/>
-    <mergeCell ref="A384:B384"/>
-    <mergeCell ref="C384:D384"/>
-    <mergeCell ref="A385:B385"/>
-    <mergeCell ref="C385:D385"/>
-    <mergeCell ref="A386:B386"/>
-    <mergeCell ref="C386:D386"/>
-    <mergeCell ref="A387:B387"/>
-    <mergeCell ref="C387:D387"/>
-    <mergeCell ref="A388:D388"/>
-    <mergeCell ref="A389:D389"/>
-    <mergeCell ref="A390:D390"/>
-    <mergeCell ref="A391:D391"/>
-    <mergeCell ref="A398:D398"/>
-    <mergeCell ref="A399:B399"/>
-    <mergeCell ref="C399:D399"/>
-    <mergeCell ref="A400:B400"/>
-    <mergeCell ref="C400:D400"/>
-    <mergeCell ref="G381:G382"/>
-    <mergeCell ref="H381:K382"/>
-    <mergeCell ref="H384:I384"/>
-    <mergeCell ref="J384:K384"/>
-    <mergeCell ref="H385:I385"/>
-    <mergeCell ref="J385:K385"/>
-    <mergeCell ref="H386:I386"/>
-    <mergeCell ref="J386:K386"/>
-    <mergeCell ref="H387:I387"/>
-    <mergeCell ref="J387:K387"/>
-    <mergeCell ref="H388:K388"/>
-    <mergeCell ref="H389:K389"/>
-    <mergeCell ref="H390:K390"/>
-    <mergeCell ref="H391:K391"/>
-    <mergeCell ref="H398:K398"/>
-    <mergeCell ref="H399:I399"/>
-    <mergeCell ref="J399:K399"/>
-    <mergeCell ref="H400:I400"/>
-    <mergeCell ref="J400:K400"/>
+    <mergeCell ref="G295:G296"/>
+    <mergeCell ref="A281:D281"/>
+    <mergeCell ref="A282:D282"/>
+    <mergeCell ref="A283:D283"/>
+    <mergeCell ref="A284:D284"/>
+    <mergeCell ref="A291:D291"/>
+    <mergeCell ref="A292:B292"/>
+    <mergeCell ref="C292:D292"/>
+    <mergeCell ref="A293:B293"/>
+    <mergeCell ref="C293:D293"/>
+    <mergeCell ref="E274:E275"/>
+    <mergeCell ref="A277:B277"/>
+    <mergeCell ref="C277:D277"/>
+    <mergeCell ref="A278:B278"/>
+    <mergeCell ref="A300:B300"/>
+    <mergeCell ref="C300:D300"/>
+    <mergeCell ref="A301:B301"/>
+    <mergeCell ref="C301:D301"/>
+    <mergeCell ref="A295:D296"/>
+    <mergeCell ref="E295:E296"/>
+    <mergeCell ref="A298:B298"/>
+    <mergeCell ref="C298:D298"/>
+    <mergeCell ref="A299:B299"/>
+    <mergeCell ref="C299:D299"/>
+    <mergeCell ref="C278:D278"/>
+    <mergeCell ref="A279:B279"/>
+    <mergeCell ref="C279:D279"/>
+    <mergeCell ref="A280:B280"/>
+    <mergeCell ref="C280:D280"/>
+    <mergeCell ref="A303:D303"/>
+    <mergeCell ref="A325:D325"/>
+    <mergeCell ref="A326:D326"/>
+    <mergeCell ref="A333:D333"/>
+    <mergeCell ref="A302:D302"/>
+    <mergeCell ref="A304:D304"/>
+    <mergeCell ref="A305:D305"/>
+    <mergeCell ref="A312:D312"/>
+    <mergeCell ref="A313:B313"/>
+    <mergeCell ref="C313:D313"/>
+    <mergeCell ref="A314:B314"/>
+    <mergeCell ref="C314:D314"/>
+    <mergeCell ref="A316:D317"/>
+    <mergeCell ref="E316:E317"/>
+    <mergeCell ref="A319:B319"/>
+    <mergeCell ref="C319:D319"/>
+    <mergeCell ref="A320:B320"/>
+    <mergeCell ref="C320:D320"/>
+    <mergeCell ref="A335:B335"/>
+    <mergeCell ref="C335:D335"/>
+    <mergeCell ref="A321:B321"/>
+    <mergeCell ref="C321:D321"/>
+    <mergeCell ref="A322:B322"/>
+    <mergeCell ref="C322:D322"/>
+    <mergeCell ref="A323:D323"/>
+    <mergeCell ref="A334:B334"/>
+    <mergeCell ref="C334:D334"/>
+    <mergeCell ref="H323:K323"/>
+    <mergeCell ref="H324:K324"/>
+    <mergeCell ref="H325:K325"/>
+    <mergeCell ref="H326:K326"/>
+    <mergeCell ref="H333:K333"/>
+    <mergeCell ref="H334:I334"/>
+    <mergeCell ref="J334:K334"/>
+    <mergeCell ref="A324:D324"/>
+    <mergeCell ref="H335:I335"/>
+    <mergeCell ref="J335:K335"/>
+    <mergeCell ref="H295:K296"/>
+    <mergeCell ref="H298:I298"/>
+    <mergeCell ref="J298:K298"/>
+    <mergeCell ref="H299:I299"/>
+    <mergeCell ref="J299:K299"/>
+    <mergeCell ref="H300:I300"/>
+    <mergeCell ref="J300:K300"/>
+    <mergeCell ref="H301:I301"/>
+    <mergeCell ref="J301:K301"/>
+    <mergeCell ref="H319:I319"/>
+    <mergeCell ref="J319:K319"/>
+    <mergeCell ref="H320:I320"/>
+    <mergeCell ref="J320:K320"/>
+    <mergeCell ref="H321:I321"/>
+    <mergeCell ref="J321:K321"/>
+    <mergeCell ref="H322:I322"/>
+    <mergeCell ref="J322:K322"/>
+    <mergeCell ref="G316:G317"/>
+    <mergeCell ref="H316:K317"/>
+    <mergeCell ref="H302:K302"/>
+    <mergeCell ref="H303:K303"/>
+    <mergeCell ref="H304:K304"/>
+    <mergeCell ref="H305:K305"/>
+    <mergeCell ref="H312:K312"/>
+    <mergeCell ref="H313:I313"/>
+    <mergeCell ref="J313:K313"/>
+    <mergeCell ref="H314:I314"/>
+    <mergeCell ref="J314:K314"/>
+    <mergeCell ref="A338:D339"/>
+    <mergeCell ref="E338:E339"/>
+    <mergeCell ref="A341:B341"/>
+    <mergeCell ref="C341:D341"/>
+    <mergeCell ref="A342:B342"/>
+    <mergeCell ref="C342:D342"/>
+    <mergeCell ref="A343:B343"/>
+    <mergeCell ref="C343:D343"/>
+    <mergeCell ref="A344:B344"/>
+    <mergeCell ref="C344:D344"/>
+    <mergeCell ref="A345:D345"/>
+    <mergeCell ref="A346:D346"/>
+    <mergeCell ref="A347:D347"/>
+    <mergeCell ref="A348:D348"/>
+    <mergeCell ref="A355:D355"/>
+    <mergeCell ref="A356:B356"/>
+    <mergeCell ref="C356:D356"/>
+    <mergeCell ref="A357:B357"/>
+    <mergeCell ref="C357:D357"/>
+    <mergeCell ref="G338:G339"/>
+    <mergeCell ref="H338:K339"/>
+    <mergeCell ref="H341:I341"/>
+    <mergeCell ref="J341:K341"/>
+    <mergeCell ref="H342:I342"/>
+    <mergeCell ref="J342:K342"/>
+    <mergeCell ref="H343:I343"/>
+    <mergeCell ref="J343:K343"/>
+    <mergeCell ref="H344:I344"/>
+    <mergeCell ref="J344:K344"/>
+    <mergeCell ref="H345:K345"/>
+    <mergeCell ref="H346:K346"/>
+    <mergeCell ref="H347:K347"/>
+    <mergeCell ref="H348:K348"/>
+    <mergeCell ref="H355:K355"/>
+    <mergeCell ref="H356:I356"/>
+    <mergeCell ref="J356:K356"/>
+    <mergeCell ref="H357:I357"/>
+    <mergeCell ref="J357:K357"/>
+    <mergeCell ref="A403:D404"/>
+    <mergeCell ref="E403:E404"/>
+    <mergeCell ref="A406:B406"/>
+    <mergeCell ref="C406:D406"/>
+    <mergeCell ref="A407:B407"/>
+    <mergeCell ref="C407:D407"/>
+    <mergeCell ref="A408:B408"/>
+    <mergeCell ref="C408:D408"/>
+    <mergeCell ref="A409:B409"/>
+    <mergeCell ref="C409:D409"/>
+    <mergeCell ref="A410:D410"/>
+    <mergeCell ref="A411:D411"/>
+    <mergeCell ref="A412:D412"/>
+    <mergeCell ref="A413:D413"/>
+    <mergeCell ref="A420:D420"/>
+    <mergeCell ref="A421:B421"/>
+    <mergeCell ref="C421:D421"/>
+    <mergeCell ref="A422:B422"/>
+    <mergeCell ref="C422:D422"/>
+    <mergeCell ref="G403:G404"/>
+    <mergeCell ref="H403:K404"/>
+    <mergeCell ref="H406:I406"/>
+    <mergeCell ref="J406:K406"/>
+    <mergeCell ref="H407:I407"/>
+    <mergeCell ref="J407:K407"/>
+    <mergeCell ref="H408:I408"/>
+    <mergeCell ref="J408:K408"/>
+    <mergeCell ref="H409:I409"/>
+    <mergeCell ref="J409:K409"/>
+    <mergeCell ref="H410:K410"/>
+    <mergeCell ref="H411:K411"/>
+    <mergeCell ref="H412:K412"/>
+    <mergeCell ref="H413:K413"/>
+    <mergeCell ref="H420:K420"/>
+    <mergeCell ref="H421:I421"/>
+    <mergeCell ref="J421:K421"/>
+    <mergeCell ref="H422:I422"/>
+    <mergeCell ref="J422:K422"/>
+    <mergeCell ref="A425:D426"/>
+    <mergeCell ref="E425:E426"/>
+    <mergeCell ref="A428:B428"/>
+    <mergeCell ref="C428:D428"/>
+    <mergeCell ref="A429:B429"/>
+    <mergeCell ref="C429:D429"/>
+    <mergeCell ref="A430:B430"/>
+    <mergeCell ref="C430:D430"/>
+    <mergeCell ref="A431:B431"/>
+    <mergeCell ref="C431:D431"/>
+    <mergeCell ref="A432:D432"/>
+    <mergeCell ref="A433:D433"/>
+    <mergeCell ref="A434:D434"/>
+    <mergeCell ref="A435:D435"/>
+    <mergeCell ref="A442:D442"/>
+    <mergeCell ref="A443:B443"/>
+    <mergeCell ref="C443:D443"/>
+    <mergeCell ref="A444:B444"/>
+    <mergeCell ref="C444:D444"/>
+    <mergeCell ref="G425:G426"/>
+    <mergeCell ref="H425:K426"/>
+    <mergeCell ref="H428:I428"/>
+    <mergeCell ref="J428:K428"/>
+    <mergeCell ref="H429:I429"/>
+    <mergeCell ref="J429:K429"/>
+    <mergeCell ref="H430:I430"/>
+    <mergeCell ref="J430:K430"/>
+    <mergeCell ref="H431:I431"/>
+    <mergeCell ref="J431:K431"/>
+    <mergeCell ref="H432:K432"/>
+    <mergeCell ref="H433:K433"/>
+    <mergeCell ref="H434:K434"/>
+    <mergeCell ref="H435:K435"/>
+    <mergeCell ref="H442:K442"/>
+    <mergeCell ref="H443:I443"/>
+    <mergeCell ref="J443:K443"/>
+    <mergeCell ref="H444:I444"/>
+    <mergeCell ref="J444:K444"/>
+    <mergeCell ref="A447:D448"/>
+    <mergeCell ref="E447:E448"/>
+    <mergeCell ref="A450:B450"/>
+    <mergeCell ref="C450:D450"/>
+    <mergeCell ref="A451:B451"/>
+    <mergeCell ref="C451:D451"/>
+    <mergeCell ref="A452:B452"/>
+    <mergeCell ref="C452:D452"/>
+    <mergeCell ref="A453:B453"/>
+    <mergeCell ref="C453:D453"/>
+    <mergeCell ref="A454:D454"/>
+    <mergeCell ref="H455:K455"/>
+    <mergeCell ref="A456:D456"/>
+    <mergeCell ref="H457:K457"/>
+    <mergeCell ref="A464:D464"/>
+    <mergeCell ref="A465:B465"/>
+    <mergeCell ref="C465:D465"/>
+    <mergeCell ref="A466:B466"/>
+    <mergeCell ref="C466:D466"/>
+    <mergeCell ref="H454:K454"/>
+    <mergeCell ref="H456:K456"/>
+    <mergeCell ref="H464:K464"/>
+    <mergeCell ref="H465:I465"/>
+    <mergeCell ref="J465:K465"/>
+    <mergeCell ref="H466:I466"/>
+    <mergeCell ref="J466:K466"/>
+    <mergeCell ref="G447:G448"/>
+    <mergeCell ref="H447:K448"/>
+    <mergeCell ref="H450:I450"/>
+    <mergeCell ref="J450:K450"/>
+    <mergeCell ref="H451:I451"/>
+    <mergeCell ref="J451:K451"/>
+    <mergeCell ref="H452:I452"/>
+    <mergeCell ref="J452:K452"/>
+    <mergeCell ref="H453:I453"/>
+    <mergeCell ref="J453:K453"/>
+    <mergeCell ref="A469:D470"/>
+    <mergeCell ref="E469:E470"/>
+    <mergeCell ref="A472:B472"/>
+    <mergeCell ref="C472:D472"/>
+    <mergeCell ref="A473:B473"/>
+    <mergeCell ref="C473:D473"/>
+    <mergeCell ref="A474:B474"/>
+    <mergeCell ref="C474:D474"/>
+    <mergeCell ref="A475:B475"/>
+    <mergeCell ref="C475:D475"/>
+    <mergeCell ref="A476:D476"/>
+    <mergeCell ref="A477:D477"/>
+    <mergeCell ref="A478:D478"/>
+    <mergeCell ref="A479:D479"/>
+    <mergeCell ref="A486:D486"/>
+    <mergeCell ref="A487:B487"/>
+    <mergeCell ref="C487:D487"/>
+    <mergeCell ref="A488:B488"/>
+    <mergeCell ref="C488:D488"/>
+    <mergeCell ref="G469:G470"/>
+    <mergeCell ref="H469:K470"/>
+    <mergeCell ref="H472:I472"/>
+    <mergeCell ref="J472:K472"/>
+    <mergeCell ref="H473:I473"/>
+    <mergeCell ref="J473:K473"/>
+    <mergeCell ref="H474:I474"/>
+    <mergeCell ref="J474:K474"/>
+    <mergeCell ref="H475:I475"/>
+    <mergeCell ref="J475:K475"/>
+    <mergeCell ref="H476:K476"/>
+    <mergeCell ref="H477:K477"/>
+    <mergeCell ref="H478:K478"/>
+    <mergeCell ref="H479:K479"/>
+    <mergeCell ref="H486:K486"/>
+    <mergeCell ref="H487:I487"/>
+    <mergeCell ref="J487:K487"/>
+    <mergeCell ref="H488:I488"/>
+    <mergeCell ref="J488:K488"/>
+    <mergeCell ref="A492:D493"/>
+    <mergeCell ref="E492:E493"/>
+    <mergeCell ref="A495:B495"/>
+    <mergeCell ref="C495:D495"/>
+    <mergeCell ref="A496:B496"/>
+    <mergeCell ref="C496:D496"/>
+    <mergeCell ref="A497:B497"/>
+    <mergeCell ref="C497:D497"/>
+    <mergeCell ref="A498:B498"/>
+    <mergeCell ref="C498:D498"/>
+    <mergeCell ref="A499:D499"/>
+    <mergeCell ref="A500:D500"/>
+    <mergeCell ref="A501:D501"/>
+    <mergeCell ref="A502:D502"/>
+    <mergeCell ref="A509:D509"/>
+    <mergeCell ref="A510:B510"/>
+    <mergeCell ref="C510:D510"/>
+    <mergeCell ref="A511:B511"/>
+    <mergeCell ref="C511:D511"/>
+    <mergeCell ref="G492:G493"/>
+    <mergeCell ref="H492:K493"/>
+    <mergeCell ref="H495:I495"/>
+    <mergeCell ref="J495:K495"/>
+    <mergeCell ref="H496:I496"/>
+    <mergeCell ref="J496:K496"/>
+    <mergeCell ref="H497:I497"/>
+    <mergeCell ref="J497:K497"/>
+    <mergeCell ref="H498:I498"/>
+    <mergeCell ref="J498:K498"/>
+    <mergeCell ref="H499:K499"/>
+    <mergeCell ref="H500:K500"/>
+    <mergeCell ref="H501:K501"/>
+    <mergeCell ref="H502:K502"/>
+    <mergeCell ref="H509:K509"/>
+    <mergeCell ref="H510:I510"/>
+    <mergeCell ref="J510:K510"/>
+    <mergeCell ref="H511:I511"/>
+    <mergeCell ref="J511:K511"/>
+    <mergeCell ref="A516:D517"/>
+    <mergeCell ref="E516:E517"/>
+    <mergeCell ref="A519:B519"/>
+    <mergeCell ref="C519:D519"/>
+    <mergeCell ref="A520:B520"/>
+    <mergeCell ref="C520:D520"/>
+    <mergeCell ref="A521:B521"/>
+    <mergeCell ref="C521:D521"/>
+    <mergeCell ref="A522:B522"/>
+    <mergeCell ref="C522:D522"/>
+    <mergeCell ref="A523:D523"/>
+    <mergeCell ref="A524:D524"/>
+    <mergeCell ref="A525:D525"/>
+    <mergeCell ref="A526:D526"/>
+    <mergeCell ref="A533:D533"/>
+    <mergeCell ref="A534:B534"/>
+    <mergeCell ref="C534:D534"/>
+    <mergeCell ref="A535:B535"/>
+    <mergeCell ref="C535:D535"/>
+    <mergeCell ref="G516:G517"/>
+    <mergeCell ref="H516:K517"/>
+    <mergeCell ref="H519:I519"/>
+    <mergeCell ref="J519:K519"/>
+    <mergeCell ref="H520:I520"/>
+    <mergeCell ref="J520:K520"/>
+    <mergeCell ref="H521:I521"/>
+    <mergeCell ref="J521:K521"/>
+    <mergeCell ref="H522:I522"/>
+    <mergeCell ref="J522:K522"/>
+    <mergeCell ref="H523:K523"/>
+    <mergeCell ref="H524:K524"/>
+    <mergeCell ref="H525:K525"/>
+    <mergeCell ref="H526:K526"/>
+    <mergeCell ref="H533:K533"/>
+    <mergeCell ref="H534:I534"/>
+    <mergeCell ref="J534:K534"/>
+    <mergeCell ref="H535:I535"/>
+    <mergeCell ref="J535:K535"/>
+    <mergeCell ref="A538:D539"/>
+    <mergeCell ref="E538:E539"/>
+    <mergeCell ref="A541:B541"/>
+    <mergeCell ref="C541:D541"/>
+    <mergeCell ref="A542:B542"/>
+    <mergeCell ref="C542:D542"/>
+    <mergeCell ref="A543:B543"/>
+    <mergeCell ref="C543:D543"/>
+    <mergeCell ref="A544:B544"/>
+    <mergeCell ref="C544:D544"/>
+    <mergeCell ref="A545:D545"/>
+    <mergeCell ref="A546:D546"/>
+    <mergeCell ref="A547:D547"/>
+    <mergeCell ref="A548:D548"/>
+    <mergeCell ref="A555:D555"/>
+    <mergeCell ref="A556:B556"/>
+    <mergeCell ref="C556:D556"/>
+    <mergeCell ref="A557:B557"/>
+    <mergeCell ref="C557:D557"/>
+    <mergeCell ref="G538:G539"/>
+    <mergeCell ref="H538:K539"/>
+    <mergeCell ref="H541:I541"/>
+    <mergeCell ref="J541:K541"/>
+    <mergeCell ref="H542:I542"/>
+    <mergeCell ref="J542:K542"/>
+    <mergeCell ref="H543:I543"/>
+    <mergeCell ref="J543:K543"/>
+    <mergeCell ref="H544:I544"/>
+    <mergeCell ref="J544:K544"/>
+    <mergeCell ref="H545:K545"/>
+    <mergeCell ref="H546:K546"/>
+    <mergeCell ref="H547:K547"/>
+    <mergeCell ref="H548:K548"/>
+    <mergeCell ref="H555:K555"/>
+    <mergeCell ref="H556:I556"/>
+    <mergeCell ref="J556:K556"/>
+    <mergeCell ref="H557:I557"/>
+    <mergeCell ref="J557:K557"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>